<commit_message>
app.r y global modular
</commit_message>
<xml_diff>
--- a/datos/CUBOgv_202516.xlsx
+++ b/datos/CUBOgv_202516.xlsx
@@ -3193,7 +3193,7 @@
         <v>202516</v>
       </c>
       <c r="F4" s="2">
-        <v>34954</v>
+        <v>34968</v>
       </c>
       <c r="G4" s="2">
         <v>35679</v>
@@ -3205,25 +3205,25 @@
         <v>223</v>
       </c>
       <c r="J4" s="2">
-        <v>60554474.030000016</v>
+        <v>60634625.23</v>
       </c>
       <c r="K4" s="2">
         <v>60566141.37</v>
       </c>
       <c r="L4" s="2">
-        <v>591</v>
+        <v>605</v>
       </c>
       <c r="M4" s="2">
         <v>1077</v>
       </c>
       <c r="N4" s="2">
-        <v>23204</v>
+        <v>23253</v>
       </c>
       <c r="O4" s="2">
         <v>24052</v>
       </c>
       <c r="P4" s="2">
-        <v>11.067575819255037</v>
+        <v>11.059110794587445</v>
       </c>
       <c r="Q4" s="2" t="s">
         <v>223</v>
@@ -3235,13 +3235,13 @@
         <v>223</v>
       </c>
       <c r="T4" s="2">
-        <v>7307275</v>
+        <v>7316804</v>
       </c>
       <c r="U4" s="2" t="s">
         <v>223</v>
       </c>
       <c r="V4" s="2">
-        <v>23183</v>
+        <v>23232</v>
       </c>
       <c r="W4" s="2" t="s">
         <v>223</v>
@@ -3253,7 +3253,7 @@
         <v>223</v>
       </c>
       <c r="Z4" s="2">
-        <v>337121</v>
+        <v>337570</v>
       </c>
       <c r="AA4" s="2" t="s">
         <v>223</v>
@@ -3277,19 +3277,19 @@
         <v>223</v>
       </c>
       <c r="AH4" s="2">
-        <v>66.38439091377238</v>
+        <v>66.49794097460536</v>
       </c>
       <c r="AI4" s="2">
         <v>67.41</v>
       </c>
       <c r="AJ4" s="2">
-        <v>25737</v>
+        <v>25787</v>
       </c>
       <c r="AK4" s="2" t="s">
         <v>223</v>
       </c>
       <c r="AL4" s="2">
-        <v>20614</v>
+        <v>20649</v>
       </c>
       <c r="AM4" s="2">
         <v>20987</v>
@@ -3301,31 +3301,31 @@
         <v>223</v>
       </c>
       <c r="AP4" s="2">
-        <v>21056</v>
+        <v>21089</v>
       </c>
       <c r="AQ4" s="2" t="s">
         <v>223</v>
       </c>
       <c r="AR4" s="2">
-        <v>16679</v>
+        <v>16711</v>
       </c>
       <c r="AS4" s="2" t="s">
         <v>223</v>
       </c>
       <c r="AT4" s="2">
-        <v>58.974652400297536</v>
+        <v>59.05113246396706</v>
       </c>
       <c r="AU4" s="2">
         <v>58.82</v>
       </c>
       <c r="AV4" s="2">
-        <v>2609.66</v>
+        <v>2607.6</v>
       </c>
       <c r="AW4" s="2">
         <v>2518.13</v>
       </c>
       <c r="AX4" s="2">
-        <v>14533</v>
+        <v>14551</v>
       </c>
       <c r="AY4" s="2" t="s">
         <v>223</v>
@@ -3379,13 +3379,13 @@
         <v>223</v>
       </c>
       <c r="BP4" s="2">
-        <v>60507985.559999995</v>
+        <v>60588136.760000005</v>
       </c>
       <c r="BQ4" s="2" t="s">
         <v>223</v>
       </c>
       <c r="BR4" s="2">
-        <v>43882494.64</v>
+        <v>43924235.74</v>
       </c>
       <c r="BS4" s="2" t="s">
         <v>223</v>
@@ -3397,43 +3397,43 @@
         <v>223</v>
       </c>
       <c r="BV4" s="2">
-        <v>43836006.17000001</v>
+        <v>43877747.27</v>
       </c>
       <c r="BW4" s="2">
         <v>43214017</v>
       </c>
       <c r="BX4" s="2">
-        <v>9100805.889999997</v>
+        <v>9121116.68</v>
       </c>
       <c r="BY4" s="2">
         <v>10842094.49</v>
       </c>
       <c r="BZ4" s="2">
-        <v>5981940.279999999</v>
+        <v>5989328.729999999</v>
       </c>
       <c r="CA4" s="2">
         <v>6510029.876</v>
       </c>
       <c r="CB4" s="2">
-        <v>119.89299332173104</v>
+        <v>119.93841382025049</v>
       </c>
       <c r="CC4" s="2" t="s">
         <v>223</v>
       </c>
       <c r="CD4" s="2">
-        <v>15082746.170000002</v>
+        <v>15110445.41</v>
       </c>
       <c r="CE4" s="2" t="s">
         <v>223</v>
       </c>
       <c r="CF4" s="2">
-        <v>8.28687493354226</v>
+        <v>8.287036967233234</v>
       </c>
       <c r="CG4" s="2" t="s">
         <v>223</v>
       </c>
       <c r="CH4" s="2">
-        <v>179.622373064864</v>
+        <v>179.62089412566283</v>
       </c>
       <c r="CI4" s="2" t="s">
         <v>223</v>
@@ -3475,43 +3475,43 @@
         <v>223</v>
       </c>
       <c r="CV4" s="2">
-        <v>2609.6566984140673</v>
+        <v>2607.6044050230075</v>
       </c>
       <c r="CW4" s="2" t="s">
         <v>223</v>
       </c>
       <c r="CX4" s="2">
-        <v>314.672254783658</v>
+        <v>314.4189566937599</v>
       </c>
       <c r="CY4" s="2" t="s">
         <v>223</v>
       </c>
       <c r="CZ4" s="2">
-        <v>21.675525998083774</v>
+        <v>21.674923719524838</v>
       </c>
       <c r="DA4" s="2" t="s">
         <v>223</v>
       </c>
       <c r="DB4" s="2">
-        <v>5611</v>
+        <v>5584</v>
       </c>
       <c r="DC4" s="2">
         <v>5403</v>
       </c>
       <c r="DD4" s="2">
-        <v>3855</v>
+        <v>3852</v>
       </c>
       <c r="DE4" s="2">
         <v>3638</v>
       </c>
       <c r="DF4" s="2">
-        <v>2284</v>
+        <v>2279</v>
       </c>
       <c r="DG4" s="2">
         <v>2024</v>
       </c>
       <c r="DH4" s="2">
-        <v>1466</v>
+        <v>1464</v>
       </c>
       <c r="DI4" s="2">
         <v>1471</v>
@@ -3529,7 +3529,7 @@
         <v>1202</v>
       </c>
       <c r="DN4" s="2">
-        <v>4350</v>
+        <v>4348</v>
       </c>
       <c r="DO4" s="2" t="s">
         <v>223</v>
@@ -3571,25 +3571,25 @@
         <v>223</v>
       </c>
       <c r="EB4" s="2">
-        <v>1410</v>
+        <v>1422</v>
       </c>
       <c r="EC4" s="2" t="s">
         <v>223</v>
       </c>
       <c r="ED4" s="2">
-        <v>1579</v>
+        <v>1591</v>
       </c>
       <c r="EE4" s="2">
         <v>2081</v>
       </c>
       <c r="EF4" s="2">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="EG4" s="2" t="s">
         <v>223</v>
       </c>
       <c r="EH4" s="2">
-        <v>39.409905163329825</v>
+        <v>39.51527924130664</v>
       </c>
       <c r="EI4" s="2" t="s">
         <v>223</v>
@@ -3601,7 +3601,7 @@
         <v>223</v>
       </c>
       <c r="EL4" s="2">
-        <v>1012</v>
+        <v>1014</v>
       </c>
       <c r="EM4" s="2">
         <v>984</v>
@@ -3613,19 +3613,19 @@
         <v>223</v>
       </c>
       <c r="EP4" s="2">
-        <v>39304</v>
+        <v>39316</v>
       </c>
       <c r="EQ4" s="2">
         <v>40019</v>
       </c>
       <c r="ER4" s="2">
-        <v>3.0938326887848566</v>
+        <v>3.0928883914945566</v>
       </c>
       <c r="ES4" s="2" t="s">
         <v>223</v>
       </c>
       <c r="ET4" s="2">
-        <v>25807</v>
+        <v>25857</v>
       </c>
       <c r="EU4" s="2" t="s">
         <v>223</v>
@@ -3637,13 +3637,13 @@
         <v>223</v>
       </c>
       <c r="EX4" s="2">
-        <v>7301655</v>
+        <v>7311184</v>
       </c>
       <c r="EY4" s="2" t="s">
         <v>223</v>
       </c>
       <c r="EZ4" s="2">
-        <v>5523390</v>
+        <v>5528419</v>
       </c>
       <c r="FA4" s="2" t="s">
         <v>223</v>
@@ -3655,31 +3655,31 @@
         <v>223</v>
       </c>
       <c r="FD4" s="2">
-        <v>5517770</v>
+        <v>5522799</v>
       </c>
       <c r="FE4" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FF4" s="2">
-        <v>1141354</v>
+        <v>1144207</v>
       </c>
       <c r="FG4" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FH4" s="2">
-        <v>643160</v>
+        <v>643950</v>
       </c>
       <c r="FI4" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FJ4" s="2">
-        <v>1784514</v>
+        <v>1788157</v>
       </c>
       <c r="FK4" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FL4" s="2">
-        <v>14.467817395970071</v>
+        <v>14.473015420889807</v>
       </c>
       <c r="FM4" s="2" t="s">
         <v>223</v>
@@ -3691,7 +3691,7 @@
         <v>223</v>
       </c>
       <c r="FP4" s="2">
-        <v>256698</v>
+        <v>256911</v>
       </c>
       <c r="FQ4" s="2" t="s">
         <v>223</v>
@@ -3703,49 +3703,49 @@
         <v>223</v>
       </c>
       <c r="FT4" s="2">
-        <v>256405</v>
+        <v>256618</v>
       </c>
       <c r="FU4" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FV4" s="2">
-        <v>505080</v>
+        <v>505659</v>
       </c>
       <c r="FW4" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FX4" s="2">
-        <v>439055</v>
+        <v>439582</v>
       </c>
       <c r="FY4" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FZ4" s="2">
-        <v>182650</v>
+        <v>182964</v>
       </c>
       <c r="GA4" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GB4" s="2">
-        <v>65732</v>
+        <v>65784</v>
       </c>
       <c r="GC4" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GD4" s="2">
-        <v>248382</v>
+        <v>248748</v>
       </c>
       <c r="GE4" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GF4" s="2">
-        <v>21.766548870884332</v>
+        <v>21.74119468455683</v>
       </c>
       <c r="GG4" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GH4" s="2">
-        <v>14.528572659886226</v>
+        <v>14.5172665892573</v>
       </c>
       <c r="GI4" s="2" t="s">
         <v>223</v>
@@ -3763,43 +3763,43 @@
         <v>223</v>
       </c>
       <c r="GN4" s="2">
-        <v>17603</v>
+        <v>17614</v>
       </c>
       <c r="GO4" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GP4" s="2">
-        <v>22596</v>
+        <v>22598</v>
       </c>
       <c r="GQ4" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GR4" s="2">
-        <v>3238</v>
+        <v>3243</v>
       </c>
       <c r="GS4" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GT4" s="2">
-        <v>12253</v>
+        <v>12257</v>
       </c>
       <c r="GU4" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GV4" s="2">
-        <v>13655</v>
+        <v>13673</v>
       </c>
       <c r="GW4" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GX4" s="2">
-        <v>6813</v>
+        <v>6827</v>
       </c>
       <c r="GY4" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GZ4" s="2">
-        <v>2655</v>
+        <v>2669</v>
       </c>
       <c r="HA4" s="2" t="s">
         <v>223</v>
@@ -3817,25 +3817,25 @@
         <v>223</v>
       </c>
       <c r="HF4" s="2">
-        <v>0.9015770914868059</v>
+        <v>0.9004911629346019</v>
       </c>
       <c r="HG4" s="2" t="s">
         <v>223</v>
       </c>
       <c r="HH4" s="2">
-        <v>357</v>
+        <v>369</v>
       </c>
       <c r="HI4" s="2" t="s">
         <v>223</v>
       </c>
       <c r="HJ4" s="2">
-        <v>6523</v>
+        <v>6538</v>
       </c>
       <c r="HK4" s="2" t="s">
         <v>223</v>
       </c>
       <c r="HL4" s="2">
-        <v>2146</v>
+        <v>2160</v>
       </c>
       <c r="HM4" s="2" t="s">
         <v>223</v>
@@ -3858,7 +3858,7 @@
         <v>202516</v>
       </c>
       <c r="F5" s="2">
-        <v>29260</v>
+        <v>29268</v>
       </c>
       <c r="G5" s="2">
         <v>29450</v>
@@ -3870,25 +3870,25 @@
         <v>223</v>
       </c>
       <c r="J5" s="2">
-        <v>46944802.56</v>
+        <v>47023695.120000005</v>
       </c>
       <c r="K5" s="2">
         <v>47526999.02</v>
       </c>
       <c r="L5" s="2">
-        <v>749</v>
+        <v>757</v>
       </c>
       <c r="M5" s="2">
         <v>593</v>
       </c>
       <c r="N5" s="2">
-        <v>18785</v>
+        <v>18835</v>
       </c>
       <c r="O5" s="2">
         <v>19340</v>
       </c>
       <c r="P5" s="2">
-        <v>11.27956337174045</v>
+        <v>11.268758526603001</v>
       </c>
       <c r="Q5" s="2" t="s">
         <v>223</v>
@@ -3900,13 +3900,13 @@
         <v>223</v>
       </c>
       <c r="T5" s="2">
-        <v>5593129</v>
+        <v>5601984</v>
       </c>
       <c r="U5" s="2" t="s">
         <v>223</v>
       </c>
       <c r="V5" s="2">
-        <v>18778</v>
+        <v>18828</v>
       </c>
       <c r="W5" s="2" t="s">
         <v>223</v>
@@ -3918,7 +3918,7 @@
         <v>223</v>
       </c>
       <c r="Z5" s="2">
-        <v>261939</v>
+        <v>262413</v>
       </c>
       <c r="AA5" s="2" t="s">
         <v>223</v>
@@ -3942,19 +3942,19 @@
         <v>223</v>
       </c>
       <c r="AH5" s="2">
-        <v>64.20027341079972</v>
+        <v>64.3535602022687</v>
       </c>
       <c r="AI5" s="2">
         <v>65.67</v>
       </c>
       <c r="AJ5" s="2">
-        <v>20527</v>
+        <v>20579</v>
       </c>
       <c r="AK5" s="2" t="s">
         <v>223</v>
       </c>
       <c r="AL5" s="2">
-        <v>16272</v>
+        <v>16314</v>
       </c>
       <c r="AM5" s="2">
         <v>16968</v>
@@ -3966,31 +3966,31 @@
         <v>223</v>
       </c>
       <c r="AP5" s="2">
-        <v>16726</v>
+        <v>16770</v>
       </c>
       <c r="AQ5" s="2" t="s">
         <v>223</v>
       </c>
       <c r="AR5" s="2">
-        <v>13414</v>
+        <v>13448</v>
       </c>
       <c r="AS5" s="2" t="s">
         <v>223</v>
       </c>
       <c r="AT5" s="2">
-        <v>55.611756664388245</v>
+        <v>55.740057400574</v>
       </c>
       <c r="AU5" s="2">
         <v>57.62</v>
       </c>
       <c r="AV5" s="2">
-        <v>2499.06</v>
+        <v>2496.61</v>
       </c>
       <c r="AW5" s="2">
         <v>2457.45</v>
       </c>
       <c r="AX5" s="2">
-        <v>11358</v>
+        <v>11386</v>
       </c>
       <c r="AY5" s="2" t="s">
         <v>223</v>
@@ -4044,13 +4044,13 @@
         <v>223</v>
       </c>
       <c r="BP5" s="2">
-        <v>46663523.41</v>
+        <v>46742415.96999999</v>
       </c>
       <c r="BQ5" s="2" t="s">
         <v>223</v>
       </c>
       <c r="BR5" s="2">
-        <v>33520360.090000007</v>
+        <v>33566657.58</v>
       </c>
       <c r="BS5" s="2" t="s">
         <v>223</v>
@@ -4062,43 +4062,43 @@
         <v>223</v>
       </c>
       <c r="BV5" s="2">
-        <v>33239080.94</v>
+        <v>33285378.429999996</v>
       </c>
       <c r="BW5" s="2">
         <v>33632982.3</v>
       </c>
       <c r="BX5" s="2">
-        <v>6692952.639999999</v>
+        <v>6708221.5</v>
       </c>
       <c r="BY5" s="2">
         <v>7803624.577</v>
       </c>
       <c r="BZ5" s="2">
-        <v>5417604.83</v>
+        <v>5430741.04</v>
       </c>
       <c r="CA5" s="2">
         <v>6090392.142</v>
       </c>
       <c r="CB5" s="2">
-        <v>119.56316425391458</v>
+        <v>119.57223639979048</v>
       </c>
       <c r="CC5" s="2" t="s">
         <v>223</v>
       </c>
       <c r="CD5" s="2">
-        <v>12110557.47</v>
+        <v>12138962.540000001</v>
       </c>
       <c r="CE5" s="2" t="s">
         <v>223</v>
       </c>
       <c r="CF5" s="2">
-        <v>8.393298734929948</v>
+        <v>8.394114499434487</v>
       </c>
       <c r="CG5" s="2" t="s">
         <v>223</v>
       </c>
       <c r="CH5" s="2">
-        <v>179.22036260350694</v>
+        <v>179.19727726903776</v>
       </c>
       <c r="CI5" s="2" t="s">
         <v>223</v>
@@ -4140,61 +4140,61 @@
         <v>223</v>
       </c>
       <c r="CV5" s="2">
-        <v>2499.0578951290927</v>
+        <v>2496.6124300504384</v>
       </c>
       <c r="CW5" s="2" t="s">
         <v>223</v>
       </c>
       <c r="CX5" s="2">
-        <v>295.868192706947</v>
+        <v>295.5529068224051</v>
       </c>
       <c r="CY5" s="2" t="s">
         <v>223</v>
       </c>
       <c r="CZ5" s="2">
-        <v>21.35279206227404</v>
+        <v>21.347966754695843</v>
       </c>
       <c r="DA5" s="2" t="s">
         <v>223</v>
       </c>
       <c r="DB5" s="2">
-        <v>4977</v>
+        <v>4943</v>
       </c>
       <c r="DC5" s="2">
         <v>4513</v>
       </c>
       <c r="DD5" s="2">
-        <v>3352</v>
+        <v>3346</v>
       </c>
       <c r="DE5" s="2">
         <v>3222</v>
       </c>
       <c r="DF5" s="2">
-        <v>2146</v>
+        <v>2144</v>
       </c>
       <c r="DG5" s="2">
         <v>1907</v>
       </c>
       <c r="DH5" s="2">
-        <v>1324</v>
+        <v>1321</v>
       </c>
       <c r="DI5" s="2">
         <v>1331</v>
       </c>
       <c r="DJ5" s="2">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="DK5" s="2">
         <v>1362</v>
       </c>
       <c r="DL5" s="2">
-        <v>1093</v>
+        <v>1094</v>
       </c>
       <c r="DM5" s="2">
         <v>1122</v>
       </c>
       <c r="DN5" s="2">
-        <v>3720</v>
+        <v>3717</v>
       </c>
       <c r="DO5" s="2" t="s">
         <v>223</v>
@@ -4236,13 +4236,13 @@
         <v>223</v>
       </c>
       <c r="EB5" s="2">
-        <v>1519</v>
+        <v>1524</v>
       </c>
       <c r="EC5" s="2" t="s">
         <v>223</v>
       </c>
       <c r="ED5" s="2">
-        <v>1659</v>
+        <v>1664</v>
       </c>
       <c r="EE5" s="2">
         <v>1537</v>
@@ -4266,7 +4266,7 @@
         <v>223</v>
       </c>
       <c r="EL5" s="2">
-        <v>853</v>
+        <v>856</v>
       </c>
       <c r="EM5" s="2">
         <v>835</v>
@@ -4278,19 +4278,19 @@
         <v>223</v>
       </c>
       <c r="EP5" s="2">
-        <v>32980</v>
+        <v>32985</v>
       </c>
       <c r="EQ5" s="2">
         <v>33265</v>
       </c>
       <c r="ER5" s="2">
-        <v>3.314129775621589</v>
+        <v>3.3166590874639987</v>
       </c>
       <c r="ES5" s="2" t="s">
         <v>223</v>
       </c>
       <c r="ET5" s="2">
-        <v>20659</v>
+        <v>20711</v>
       </c>
       <c r="EU5" s="2" t="s">
         <v>223</v>
@@ -4302,13 +4302,13 @@
         <v>223</v>
       </c>
       <c r="EX5" s="2">
-        <v>5557884</v>
+        <v>5566739</v>
       </c>
       <c r="EY5" s="2" t="s">
         <v>223</v>
       </c>
       <c r="EZ5" s="2">
-        <v>4172347</v>
+        <v>4177854</v>
       </c>
       <c r="FA5" s="2" t="s">
         <v>223</v>
@@ -4320,31 +4320,31 @@
         <v>223</v>
       </c>
       <c r="FD5" s="2">
-        <v>4137102</v>
+        <v>4142609</v>
       </c>
       <c r="FE5" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FF5" s="2">
-        <v>830622</v>
+        <v>832530</v>
       </c>
       <c r="FG5" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FH5" s="2">
-        <v>590160</v>
+        <v>591600</v>
       </c>
       <c r="FI5" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FJ5" s="2">
-        <v>1420782</v>
+        <v>1424130</v>
       </c>
       <c r="FK5" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FL5" s="2">
-        <v>14.245074318198025</v>
+        <v>14.244770714986803</v>
       </c>
       <c r="FM5" s="2" t="s">
         <v>223</v>
@@ -4356,7 +4356,7 @@
         <v>223</v>
       </c>
       <c r="FP5" s="2">
-        <v>192646</v>
+        <v>192909</v>
       </c>
       <c r="FQ5" s="2" t="s">
         <v>223</v>
@@ -4368,49 +4368,49 @@
         <v>223</v>
       </c>
       <c r="FT5" s="2">
-        <v>192161</v>
+        <v>192424</v>
       </c>
       <c r="FU5" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FV5" s="2">
-        <v>392636</v>
+        <v>393272</v>
       </c>
       <c r="FW5" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FX5" s="2">
-        <v>333679</v>
+        <v>334204</v>
       </c>
       <c r="FY5" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FZ5" s="2">
-        <v>141518</v>
+        <v>141780</v>
       </c>
       <c r="GA5" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GB5" s="2">
-        <v>58472</v>
+        <v>58583</v>
       </c>
       <c r="GC5" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GD5" s="2">
-        <v>199990</v>
+        <v>200363</v>
       </c>
       <c r="GE5" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GF5" s="2">
-        <v>20.901570401916423</v>
+        <v>20.87953278470932</v>
       </c>
       <c r="GG5" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GH5" s="2">
-        <v>13.944051104604737</v>
+        <v>13.932200690204407</v>
       </c>
       <c r="GI5" s="2" t="s">
         <v>223</v>
@@ -4428,43 +4428,43 @@
         <v>223</v>
       </c>
       <c r="GN5" s="2">
-        <v>15856</v>
+        <v>15861</v>
       </c>
       <c r="GO5" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GP5" s="2">
-        <v>19087</v>
+        <v>19088</v>
       </c>
       <c r="GQ5" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GR5" s="2">
-        <v>3389</v>
+        <v>3388</v>
       </c>
       <c r="GS5" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GT5" s="2">
-        <v>9412</v>
+        <v>9417</v>
       </c>
       <c r="GU5" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GV5" s="2">
-        <v>11380</v>
+        <v>11404</v>
       </c>
       <c r="GW5" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GX5" s="2">
-        <v>4867</v>
+        <v>4885</v>
       </c>
       <c r="GY5" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GZ5" s="2">
-        <v>2458</v>
+        <v>2466</v>
       </c>
       <c r="HA5" s="2" t="s">
         <v>223</v>
@@ -4482,25 +4482,25 @@
         <v>223</v>
       </c>
       <c r="HF5" s="2">
-        <v>0.8870226051599787</v>
+        <v>0.8859060402684564</v>
       </c>
       <c r="HG5" s="2" t="s">
         <v>223</v>
       </c>
       <c r="HH5" s="2">
-        <v>561</v>
+        <v>566</v>
       </c>
       <c r="HI5" s="2" t="s">
         <v>223</v>
       </c>
       <c r="HJ5" s="2">
-        <v>5368</v>
+        <v>5384</v>
       </c>
       <c r="HK5" s="2" t="s">
         <v>223</v>
       </c>
       <c r="HL5" s="2">
-        <v>2056</v>
+        <v>2062</v>
       </c>
       <c r="HM5" s="2" t="s">
         <v>223</v>
@@ -5188,7 +5188,7 @@
         <v>202516</v>
       </c>
       <c r="F7" s="2">
-        <v>20675</v>
+        <v>20684</v>
       </c>
       <c r="G7" s="2">
         <v>21018</v>
@@ -5200,25 +5200,25 @@
         <v>223</v>
       </c>
       <c r="J7" s="2">
-        <v>33740533.809999995</v>
+        <v>33784180.72</v>
       </c>
       <c r="K7" s="2">
         <v>33526311.57</v>
       </c>
       <c r="L7" s="2">
-        <v>613</v>
+        <v>622</v>
       </c>
       <c r="M7" s="2">
         <v>526</v>
       </c>
       <c r="N7" s="2">
-        <v>14617</v>
+        <v>14647</v>
       </c>
       <c r="O7" s="2">
         <v>14463</v>
       </c>
       <c r="P7" s="2">
-        <v>12.319762510602207</v>
+        <v>12.303909098617824</v>
       </c>
       <c r="Q7" s="2" t="s">
         <v>223</v>
@@ -5230,13 +5230,13 @@
         <v>223</v>
       </c>
       <c r="T7" s="2">
-        <v>4100351</v>
+        <v>4105590</v>
       </c>
       <c r="U7" s="2" t="s">
         <v>223</v>
       </c>
       <c r="V7" s="2">
-        <v>14612</v>
+        <v>14642</v>
       </c>
       <c r="W7" s="2" t="s">
         <v>223</v>
@@ -5248,7 +5248,7 @@
         <v>223</v>
       </c>
       <c r="Z7" s="2">
-        <v>204784</v>
+        <v>205079</v>
       </c>
       <c r="AA7" s="2" t="s">
         <v>223</v>
@@ -5272,19 +5272,19 @@
         <v>223</v>
       </c>
       <c r="AH7" s="2">
-        <v>70.69891172914147</v>
+        <v>70.8131889383098</v>
       </c>
       <c r="AI7" s="2">
         <v>68.81</v>
       </c>
       <c r="AJ7" s="2">
-        <v>15965</v>
+        <v>16000</v>
       </c>
       <c r="AK7" s="2" t="s">
         <v>223</v>
       </c>
       <c r="AL7" s="2">
-        <v>12822</v>
+        <v>12843</v>
       </c>
       <c r="AM7" s="2">
         <v>12760</v>
@@ -5296,31 +5296,31 @@
         <v>223</v>
       </c>
       <c r="AP7" s="2">
-        <v>10559</v>
+        <v>10574</v>
       </c>
       <c r="AQ7" s="2" t="s">
         <v>223</v>
       </c>
       <c r="AR7" s="2">
-        <v>12087</v>
+        <v>12116</v>
       </c>
       <c r="AS7" s="2" t="s">
         <v>223</v>
       </c>
       <c r="AT7" s="2">
-        <v>62.016928657799276</v>
+        <v>62.091471668922836</v>
       </c>
       <c r="AU7" s="2">
         <v>60.71</v>
       </c>
       <c r="AV7" s="2">
-        <v>2308.31</v>
+        <v>2306.56</v>
       </c>
       <c r="AW7" s="2">
         <v>2318.07</v>
       </c>
       <c r="AX7" s="2">
-        <v>8030</v>
+        <v>8045</v>
       </c>
       <c r="AY7" s="2" t="s">
         <v>223</v>
@@ -5374,13 +5374,13 @@
         <v>223</v>
       </c>
       <c r="BP7" s="2">
-        <v>33726857.06</v>
+        <v>33770503.970000006</v>
       </c>
       <c r="BQ7" s="2" t="s">
         <v>223</v>
       </c>
       <c r="BR7" s="2">
-        <v>18955954.520000003</v>
+        <v>18965762.490000006</v>
       </c>
       <c r="BS7" s="2" t="s">
         <v>223</v>
@@ -5392,43 +5392,43 @@
         <v>223</v>
       </c>
       <c r="BV7" s="2">
-        <v>18942277.770000003</v>
+        <v>18952085.740000006</v>
       </c>
       <c r="BW7" s="2">
         <v>18151682.69</v>
       </c>
       <c r="BX7" s="2">
-        <v>8870662.85</v>
+        <v>8890079.85</v>
       </c>
       <c r="BY7" s="2">
         <v>9759100.812</v>
       </c>
       <c r="BZ7" s="2">
-        <v>4842563.649999999</v>
+        <v>4851308.12</v>
       </c>
       <c r="CA7" s="2">
         <v>5615528.068</v>
       </c>
       <c r="CB7" s="2">
-        <v>79.44014609315586</v>
+        <v>79.39411484636625</v>
       </c>
       <c r="CC7" s="2" t="s">
         <v>223</v>
       </c>
       <c r="CD7" s="2">
-        <v>13713226.499999998</v>
+        <v>13741387.969999999</v>
       </c>
       <c r="CE7" s="2" t="s">
         <v>223</v>
       </c>
       <c r="CF7" s="2">
-        <v>8.22869403375467</v>
+        <v>8.228824777924732</v>
       </c>
       <c r="CG7" s="2" t="s">
         <v>223</v>
       </c>
       <c r="CH7" s="2">
-        <v>164.761572241972</v>
+        <v>164.7373973931997</v>
       </c>
       <c r="CI7" s="2" t="s">
         <v>223</v>
@@ -5470,49 +5470,49 @@
         <v>223</v>
       </c>
       <c r="CV7" s="2">
-        <v>2308.307710884586</v>
+        <v>2306.5597542158803</v>
       </c>
       <c r="CW7" s="2" t="s">
         <v>223</v>
       </c>
       <c r="CX7" s="2">
-        <v>280.4043921461312</v>
+        <v>280.1877517580392</v>
       </c>
       <c r="CY7" s="2" t="s">
         <v>223</v>
       </c>
       <c r="CZ7" s="2">
-        <v>20.02280939917181</v>
+        <v>20.01955344038151</v>
       </c>
       <c r="DA7" s="2" t="s">
         <v>223</v>
       </c>
       <c r="DB7" s="2">
-        <v>2828</v>
+        <v>2813</v>
       </c>
       <c r="DC7" s="2">
         <v>3067</v>
       </c>
       <c r="DD7" s="2">
-        <v>1834</v>
+        <v>1830</v>
       </c>
       <c r="DE7" s="2">
         <v>1856</v>
       </c>
       <c r="DF7" s="2">
-        <v>1396</v>
+        <v>1394</v>
       </c>
       <c r="DG7" s="2">
         <v>1299</v>
       </c>
       <c r="DH7" s="2">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="DI7" s="2">
         <v>894</v>
       </c>
       <c r="DJ7" s="2">
-        <v>1044</v>
+        <v>1042</v>
       </c>
       <c r="DK7" s="2">
         <v>1069</v>
@@ -5524,7 +5524,7 @@
         <v>946</v>
       </c>
       <c r="DN7" s="2">
-        <v>2905</v>
+        <v>2902</v>
       </c>
       <c r="DO7" s="2" t="s">
         <v>223</v>
@@ -5566,13 +5566,13 @@
         <v>223</v>
       </c>
       <c r="EB7" s="2">
-        <v>1116</v>
+        <v>1122</v>
       </c>
       <c r="EC7" s="2" t="s">
         <v>223</v>
       </c>
       <c r="ED7" s="2">
-        <v>1217</v>
+        <v>1223</v>
       </c>
       <c r="EE7" s="2">
         <v>1147</v>
@@ -5596,7 +5596,7 @@
         <v>223</v>
       </c>
       <c r="EL7" s="2">
-        <v>577</v>
+        <v>580</v>
       </c>
       <c r="EM7" s="2">
         <v>556</v>
@@ -5608,19 +5608,19 @@
         <v>223</v>
       </c>
       <c r="EP7" s="2">
-        <v>23580</v>
+        <v>23586</v>
       </c>
       <c r="EQ7" s="2">
         <v>23927</v>
       </c>
       <c r="ER7" s="2">
-        <v>3.9567430025445294</v>
+        <v>3.955736453828542</v>
       </c>
       <c r="ES7" s="2" t="s">
         <v>223</v>
       </c>
       <c r="ET7" s="2">
-        <v>15980</v>
+        <v>16015</v>
       </c>
       <c r="EU7" s="2" t="s">
         <v>223</v>
@@ -5632,13 +5632,13 @@
         <v>223</v>
       </c>
       <c r="EX7" s="2">
-        <v>4098671</v>
+        <v>4103910</v>
       </c>
       <c r="EY7" s="2" t="s">
         <v>223</v>
       </c>
       <c r="EZ7" s="2">
-        <v>2385816</v>
+        <v>2386980</v>
       </c>
       <c r="FA7" s="2" t="s">
         <v>223</v>
@@ -5650,31 +5650,31 @@
         <v>223</v>
       </c>
       <c r="FD7" s="2">
-        <v>2384136</v>
+        <v>2385300</v>
       </c>
       <c r="FE7" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FF7" s="2">
-        <v>1190794</v>
+        <v>1193615</v>
       </c>
       <c r="FG7" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FH7" s="2">
-        <v>524080</v>
+        <v>524995</v>
       </c>
       <c r="FI7" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FJ7" s="2">
-        <v>1714874</v>
+        <v>1718610</v>
       </c>
       <c r="FK7" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FL7" s="2">
-        <v>9.654040576461696</v>
+        <v>9.648293284765877</v>
       </c>
       <c r="FM7" s="2" t="s">
         <v>223</v>
@@ -5686,7 +5686,7 @@
         <v>223</v>
       </c>
       <c r="FP7" s="2">
-        <v>106673</v>
+        <v>106744</v>
       </c>
       <c r="FQ7" s="2" t="s">
         <v>223</v>
@@ -5698,49 +5698,49 @@
         <v>223</v>
       </c>
       <c r="FT7" s="2">
-        <v>106575</v>
+        <v>106646</v>
       </c>
       <c r="FU7" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FV7" s="2">
-        <v>424729</v>
+        <v>425518</v>
       </c>
       <c r="FW7" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FX7" s="2">
-        <v>369607</v>
+        <v>370311</v>
       </c>
       <c r="FY7" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FZ7" s="2">
-        <v>263032</v>
+        <v>263665</v>
       </c>
       <c r="GA7" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GB7" s="2">
-        <v>55024</v>
+        <v>55109</v>
       </c>
       <c r="GC7" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GD7" s="2">
-        <v>318056</v>
+        <v>318774</v>
       </c>
       <c r="GE7" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GF7" s="2">
-        <v>29.057193678593418</v>
+        <v>29.052024305318497</v>
       </c>
       <c r="GG7" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GH7" s="2">
-        <v>14.009988369706505</v>
+        <v>14.001433740697754</v>
       </c>
       <c r="GI7" s="2" t="s">
         <v>223</v>
@@ -5758,7 +5758,7 @@
         <v>223</v>
       </c>
       <c r="GN7" s="2">
-        <v>11432</v>
+        <v>11438</v>
       </c>
       <c r="GO7" s="2" t="s">
         <v>223</v>
@@ -5770,31 +5770,31 @@
         <v>223</v>
       </c>
       <c r="GR7" s="2">
-        <v>6782</v>
+        <v>6786</v>
       </c>
       <c r="GS7" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GT7" s="2">
-        <v>7259</v>
+        <v>7261</v>
       </c>
       <c r="GU7" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GV7" s="2">
-        <v>5489</v>
+        <v>5494</v>
       </c>
       <c r="GW7" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GX7" s="2">
-        <v>4303</v>
+        <v>4311</v>
       </c>
       <c r="GY7" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GZ7" s="2">
-        <v>4752</v>
+        <v>4768</v>
       </c>
       <c r="HA7" s="2" t="s">
         <v>223</v>
@@ -5812,13 +5812,13 @@
         <v>223</v>
       </c>
       <c r="HF7" s="2">
-        <v>0.8077596996245306</v>
+        <v>0.8066812363409304</v>
       </c>
       <c r="HG7" s="2" t="s">
         <v>223</v>
       </c>
       <c r="HH7" s="2">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="HI7" s="2" t="s">
         <v>223</v>
@@ -5830,7 +5830,7 @@
         <v>223</v>
       </c>
       <c r="HL7" s="2">
-        <v>4057</v>
+        <v>4071</v>
       </c>
       <c r="HM7" s="2" t="s">
         <v>223</v>
@@ -5853,7 +5853,7 @@
         <v>202516</v>
       </c>
       <c r="F8" s="2">
-        <v>21462</v>
+        <v>21466</v>
       </c>
       <c r="G8" s="2">
         <v>21636</v>
@@ -5865,25 +5865,25 @@
         <v>223</v>
       </c>
       <c r="J8" s="2">
-        <v>35459348.72</v>
+        <v>35485611.41</v>
       </c>
       <c r="K8" s="2">
         <v>35221198.83</v>
       </c>
       <c r="L8" s="2">
-        <v>486</v>
+        <v>490</v>
       </c>
       <c r="M8" s="2">
         <v>392</v>
       </c>
       <c r="N8" s="2">
-        <v>14577</v>
+        <v>14592</v>
       </c>
       <c r="O8" s="2">
         <v>14581</v>
       </c>
       <c r="P8" s="2">
-        <v>12.087822062016139</v>
+        <v>12.085841831510832</v>
       </c>
       <c r="Q8" s="2" t="s">
         <v>223</v>
@@ -5895,13 +5895,13 @@
         <v>223</v>
       </c>
       <c r="T8" s="2">
-        <v>4232184</v>
+        <v>4235446</v>
       </c>
       <c r="U8" s="2" t="s">
         <v>223</v>
       </c>
       <c r="V8" s="2">
-        <v>14572</v>
+        <v>14587</v>
       </c>
       <c r="W8" s="2" t="s">
         <v>223</v>
@@ -5913,7 +5913,7 @@
         <v>223</v>
       </c>
       <c r="Z8" s="2">
-        <v>205966</v>
+        <v>206097</v>
       </c>
       <c r="AA8" s="2" t="s">
         <v>223</v>
@@ -5937,19 +5937,19 @@
         <v>223</v>
       </c>
       <c r="AH8" s="2">
-        <v>67.92004473022085</v>
+        <v>67.97726637473214</v>
       </c>
       <c r="AI8" s="2">
         <v>67.39</v>
       </c>
       <c r="AJ8" s="2">
-        <v>15915</v>
+        <v>15930</v>
       </c>
       <c r="AK8" s="2" t="s">
         <v>223</v>
       </c>
       <c r="AL8" s="2">
-        <v>12722</v>
+        <v>12733</v>
       </c>
       <c r="AM8" s="2">
         <v>12830</v>
@@ -5961,31 +5961,31 @@
         <v>223</v>
       </c>
       <c r="AP8" s="2">
-        <v>12657</v>
+        <v>12671</v>
       </c>
       <c r="AQ8" s="2" t="s">
         <v>223</v>
       </c>
       <c r="AR8" s="2">
-        <v>10673</v>
+        <v>10683</v>
       </c>
       <c r="AS8" s="2" t="s">
         <v>223</v>
       </c>
       <c r="AT8" s="2">
-        <v>59.27686142950331</v>
+        <v>59.31705953601043</v>
       </c>
       <c r="AU8" s="2">
         <v>59.3</v>
       </c>
       <c r="AV8" s="2">
-        <v>2432.55</v>
+        <v>2431.85</v>
       </c>
       <c r="AW8" s="2">
         <v>2415.55</v>
       </c>
       <c r="AX8" s="2">
-        <v>8755</v>
+        <v>8764</v>
       </c>
       <c r="AY8" s="2" t="s">
         <v>223</v>
@@ -6039,13 +6039,13 @@
         <v>223</v>
       </c>
       <c r="BP8" s="2">
-        <v>35450192.00999999</v>
+        <v>35476454.699999996</v>
       </c>
       <c r="BQ8" s="2" t="s">
         <v>223</v>
       </c>
       <c r="BR8" s="2">
-        <v>24689832.749999996</v>
+        <v>24706085.66</v>
       </c>
       <c r="BS8" s="2" t="s">
         <v>223</v>
@@ -6057,43 +6057,43 @@
         <v>223</v>
       </c>
       <c r="BV8" s="2">
-        <v>24680676.04</v>
+        <v>24696928.95</v>
       </c>
       <c r="BW8" s="2">
         <v>23910764.66</v>
       </c>
       <c r="BX8" s="2">
-        <v>5647681.58</v>
+        <v>5654722.140000001</v>
       </c>
       <c r="BY8" s="2">
         <v>6755385.786</v>
       </c>
       <c r="BZ8" s="2">
-        <v>4082788.87</v>
+        <v>4084793.09</v>
       </c>
       <c r="CA8" s="2">
         <v>4555048.383</v>
       </c>
       <c r="CB8" s="2">
-        <v>118.88059997921395</v>
+        <v>118.87061100819702</v>
       </c>
       <c r="CC8" s="2" t="s">
         <v>223</v>
       </c>
       <c r="CD8" s="2">
-        <v>9730470.45</v>
+        <v>9739515.23</v>
       </c>
       <c r="CE8" s="2" t="s">
         <v>223</v>
       </c>
       <c r="CF8" s="2">
-        <v>8.378498836534517</v>
+        <v>8.378246685236926</v>
       </c>
       <c r="CG8" s="2" t="s">
         <v>223</v>
       </c>
       <c r="CH8" s="2">
-        <v>172.1611757280328</v>
+        <v>172.1791749030796</v>
       </c>
       <c r="CI8" s="2" t="s">
         <v>223</v>
@@ -6135,25 +6135,25 @@
         <v>223</v>
       </c>
       <c r="CV8" s="2">
-        <v>2432.5546216642656</v>
+        <v>2431.8538521107453</v>
       </c>
       <c r="CW8" s="2" t="s">
         <v>223</v>
       </c>
       <c r="CX8" s="2">
-        <v>290.2586266035535</v>
+        <v>290.18379934210526</v>
       </c>
       <c r="CY8" s="2" t="s">
         <v>223</v>
       </c>
       <c r="CZ8" s="2">
-        <v>20.547973937445985</v>
+        <v>20.55074067065508</v>
       </c>
       <c r="DA8" s="2" t="s">
         <v>223</v>
       </c>
       <c r="DB8" s="2">
-        <v>3280</v>
+        <v>3271</v>
       </c>
       <c r="DC8" s="2">
         <v>3326</v>
@@ -6165,7 +6165,7 @@
         <v>2081</v>
       </c>
       <c r="DF8" s="2">
-        <v>1412</v>
+        <v>1410</v>
       </c>
       <c r="DG8" s="2">
         <v>1305</v>
@@ -6231,13 +6231,13 @@
         <v>223</v>
       </c>
       <c r="EB8" s="2">
-        <v>1043</v>
+        <v>1047</v>
       </c>
       <c r="EC8" s="2" t="s">
         <v>223</v>
       </c>
       <c r="ED8" s="2">
-        <v>1160</v>
+        <v>1164</v>
       </c>
       <c r="EE8" s="2">
         <v>1107</v>
@@ -6273,19 +6273,19 @@
         <v>223</v>
       </c>
       <c r="EP8" s="2">
-        <v>24413</v>
+        <v>24417</v>
       </c>
       <c r="EQ8" s="2">
         <v>24638</v>
       </c>
       <c r="ER8" s="2">
-        <v>3.551386556342932</v>
+        <v>3.5508047671704137</v>
       </c>
       <c r="ES8" s="2" t="s">
         <v>223</v>
       </c>
       <c r="ET8" s="2">
-        <v>15926</v>
+        <v>15941</v>
       </c>
       <c r="EU8" s="2" t="s">
         <v>223</v>
@@ -6297,13 +6297,13 @@
         <v>223</v>
       </c>
       <c r="EX8" s="2">
-        <v>4231100</v>
+        <v>4234362</v>
       </c>
       <c r="EY8" s="2" t="s">
         <v>223</v>
       </c>
       <c r="EZ8" s="2">
-        <v>3093111</v>
+        <v>3095183</v>
       </c>
       <c r="FA8" s="2" t="s">
         <v>223</v>
@@ -6315,31 +6315,31 @@
         <v>223</v>
       </c>
       <c r="FD8" s="2">
-        <v>3092027</v>
+        <v>3094099</v>
       </c>
       <c r="FE8" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FF8" s="2">
-        <v>700364</v>
+        <v>701350</v>
       </c>
       <c r="FG8" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FH8" s="2">
-        <v>438709</v>
+        <v>438913</v>
       </c>
       <c r="FI8" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FJ8" s="2">
-        <v>1139073</v>
+        <v>1140263</v>
       </c>
       <c r="FK8" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FL8" s="2">
-        <v>14.188770840527429</v>
+        <v>14.188005614307775</v>
       </c>
       <c r="FM8" s="2" t="s">
         <v>223</v>
@@ -6351,7 +6351,7 @@
         <v>223</v>
       </c>
       <c r="FP8" s="2">
-        <v>143650</v>
+        <v>143722</v>
       </c>
       <c r="FQ8" s="2" t="s">
         <v>223</v>
@@ -6363,49 +6363,49 @@
         <v>223</v>
       </c>
       <c r="FT8" s="2">
-        <v>143580</v>
+        <v>143652</v>
       </c>
       <c r="FU8" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FV8" s="2">
-        <v>298284</v>
+        <v>298523</v>
       </c>
       <c r="FW8" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FX8" s="2">
-        <v>253308</v>
+        <v>253517</v>
       </c>
       <c r="FY8" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FZ8" s="2">
-        <v>109728</v>
+        <v>109865</v>
       </c>
       <c r="GA8" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GB8" s="2">
-        <v>44906</v>
+        <v>44936</v>
       </c>
       <c r="GC8" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GD8" s="2">
-        <v>154634</v>
+        <v>154801</v>
       </c>
       <c r="GE8" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GF8" s="2">
-        <v>20.462166426562394</v>
+        <v>20.45799067982456</v>
       </c>
       <c r="GG8" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GH8" s="2">
-        <v>14.129519105440076</v>
+        <v>14.123972039473685</v>
       </c>
       <c r="GI8" s="2" t="s">
         <v>223</v>
@@ -6423,43 +6423,43 @@
         <v>223</v>
       </c>
       <c r="GN8" s="2">
-        <v>11327</v>
+        <v>11331</v>
       </c>
       <c r="GO8" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GP8" s="2">
-        <v>13014</v>
+        <v>13017</v>
       </c>
       <c r="GQ8" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GR8" s="2">
-        <v>3195</v>
+        <v>3197</v>
       </c>
       <c r="GS8" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GT8" s="2">
-        <v>7337</v>
+        <v>7336</v>
       </c>
       <c r="GU8" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GV8" s="2">
-        <v>8205</v>
+        <v>8213</v>
       </c>
       <c r="GW8" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GX8" s="2">
-        <v>4049</v>
+        <v>4053</v>
       </c>
       <c r="GY8" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GZ8" s="2">
-        <v>2254</v>
+        <v>2257</v>
       </c>
       <c r="HA8" s="2" t="s">
         <v>223</v>
@@ -6477,25 +6477,25 @@
         <v>223</v>
       </c>
       <c r="HF8" s="2">
-        <v>0.855016953409519</v>
+        <v>0.8547142588294335</v>
       </c>
       <c r="HG8" s="2" t="s">
         <v>223</v>
       </c>
       <c r="HH8" s="2">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="HI8" s="2" t="s">
         <v>223</v>
       </c>
       <c r="HJ8" s="2">
-        <v>3902</v>
+        <v>3907</v>
       </c>
       <c r="HK8" s="2" t="s">
         <v>223</v>
       </c>
       <c r="HL8" s="2">
-        <v>1918</v>
+        <v>1919</v>
       </c>
       <c r="HM8" s="2" t="s">
         <v>223</v>
@@ -17823,7 +17823,7 @@
         <v>202516</v>
       </c>
       <c r="F26" s="2">
-        <v>28852</v>
+        <v>28858</v>
       </c>
       <c r="G26" s="2">
         <v>28607</v>
@@ -17835,25 +17835,25 @@
         <v>223</v>
       </c>
       <c r="J26" s="2">
-        <v>48045790.62999999</v>
+        <v>48141889.85</v>
       </c>
       <c r="K26" s="2">
         <v>40956426.69</v>
       </c>
       <c r="L26" s="2">
-        <v>857</v>
+        <v>863</v>
       </c>
       <c r="M26" s="2">
         <v>255</v>
       </c>
       <c r="N26" s="2">
-        <v>18947</v>
+        <v>18994</v>
       </c>
       <c r="O26" s="2">
         <v>16477</v>
       </c>
       <c r="P26" s="2">
-        <v>12.386505116759285</v>
+        <v>12.384248717248079</v>
       </c>
       <c r="Q26" s="2" t="s">
         <v>223</v>
@@ -17865,13 +17865,13 @@
         <v>223</v>
       </c>
       <c r="T26" s="2">
-        <v>5761257</v>
+        <v>5772640</v>
       </c>
       <c r="U26" s="2" t="s">
         <v>223</v>
       </c>
       <c r="V26" s="2">
-        <v>18941</v>
+        <v>18988</v>
       </c>
       <c r="W26" s="2" t="s">
         <v>223</v>
@@ -17883,7 +17883,7 @@
         <v>223</v>
       </c>
       <c r="Z26" s="2">
-        <v>267438</v>
+        <v>268026</v>
       </c>
       <c r="AA26" s="2" t="s">
         <v>223</v>
@@ -17907,19 +17907,19 @@
         <v>223</v>
       </c>
       <c r="AH26" s="2">
-        <v>65.66962428947734</v>
+        <v>65.81883706424561</v>
       </c>
       <c r="AI26" s="2">
         <v>57.6</v>
       </c>
       <c r="AJ26" s="2">
-        <v>20857</v>
+        <v>20909</v>
       </c>
       <c r="AK26" s="2" t="s">
         <v>223</v>
       </c>
       <c r="AL26" s="2">
-        <v>16334</v>
+        <v>16375</v>
       </c>
       <c r="AM26" s="2">
         <v>14455</v>
@@ -17931,31 +17931,31 @@
         <v>223</v>
       </c>
       <c r="AP26" s="2">
-        <v>16687</v>
+        <v>16722</v>
       </c>
       <c r="AQ26" s="2" t="s">
         <v>223</v>
       </c>
       <c r="AR26" s="2">
-        <v>13552</v>
+        <v>13587</v>
       </c>
       <c r="AS26" s="2" t="s">
         <v>223</v>
       </c>
       <c r="AT26" s="2">
-        <v>56.61305975322335</v>
+        <v>56.74336405849332</v>
       </c>
       <c r="AU26" s="2">
         <v>50.53</v>
       </c>
       <c r="AV26" s="2">
-        <v>2535.8</v>
+        <v>2534.58</v>
       </c>
       <c r="AW26" s="2">
         <v>2485.67</v>
       </c>
       <c r="AX26" s="2">
-        <v>11300</v>
+        <v>11323</v>
       </c>
       <c r="AY26" s="2" t="s">
         <v>223</v>
@@ -18009,13 +18009,13 @@
         <v>223</v>
       </c>
       <c r="BP26" s="2">
-        <v>48018978.13999999</v>
+        <v>48115077.35999999</v>
       </c>
       <c r="BQ26" s="2" t="s">
         <v>223</v>
       </c>
       <c r="BR26" s="2">
-        <v>34170788.2</v>
+        <v>34223832.580000006</v>
       </c>
       <c r="BS26" s="2" t="s">
         <v>223</v>
@@ -18027,43 +18027,43 @@
         <v>223</v>
       </c>
       <c r="BV26" s="2">
-        <v>34143975.71</v>
+        <v>34197020.09</v>
       </c>
       <c r="BW26" s="2">
         <v>28940776.22</v>
       </c>
       <c r="BX26" s="2">
-        <v>7069756.700000001</v>
+        <v>7092148.340000001</v>
       </c>
       <c r="BY26" s="2">
         <v>6666897.772</v>
       </c>
       <c r="BZ26" s="2">
-        <v>5498036.209999999</v>
+        <v>5514789.409999999</v>
       </c>
       <c r="CA26" s="2">
         <v>5348752.695</v>
       </c>
       <c r="CB26" s="2">
-        <v>98.07304914492401</v>
+        <v>98.03527797632502</v>
       </c>
       <c r="CC26" s="2" t="s">
         <v>223</v>
       </c>
       <c r="CD26" s="2">
-        <v>12567792.91</v>
+        <v>12606937.75</v>
       </c>
       <c r="CE26" s="2" t="s">
         <v>223</v>
       </c>
       <c r="CF26" s="2">
-        <v>8.339463181385588</v>
+        <v>8.339666054006486</v>
       </c>
       <c r="CG26" s="2" t="s">
         <v>223</v>
       </c>
       <c r="CH26" s="2">
-        <v>179.6520712464197</v>
+        <v>179.6164918701917</v>
       </c>
       <c r="CI26" s="2" t="s">
         <v>223</v>
@@ -18105,37 +18105,37 @@
         <v>223</v>
       </c>
       <c r="CV26" s="2">
-        <v>2535.799368237715</v>
+        <v>2534.5840712856693</v>
       </c>
       <c r="CW26" s="2" t="s">
         <v>223</v>
       </c>
       <c r="CX26" s="2">
-        <v>303.8963952076846</v>
+        <v>303.74370853953883</v>
       </c>
       <c r="CY26" s="2" t="s">
         <v>223</v>
       </c>
       <c r="CZ26" s="2">
-        <v>21.542402351199158</v>
+        <v>21.537612022714214</v>
       </c>
       <c r="DA26" s="2" t="s">
         <v>223</v>
       </c>
       <c r="DB26" s="2">
-        <v>4453</v>
+        <v>4417</v>
       </c>
       <c r="DC26" s="2">
         <v>5640</v>
       </c>
       <c r="DD26" s="2">
-        <v>3225</v>
+        <v>3221</v>
       </c>
       <c r="DE26" s="2">
         <v>3814</v>
       </c>
       <c r="DF26" s="2">
-        <v>2227</v>
+        <v>2226</v>
       </c>
       <c r="DG26" s="2">
         <v>2218</v>
@@ -18201,25 +18201,25 @@
         <v>223</v>
       </c>
       <c r="EB26" s="2">
-        <v>1548</v>
+        <v>1554</v>
       </c>
       <c r="EC26" s="2" t="s">
         <v>223</v>
       </c>
       <c r="ED26" s="2">
-        <v>1699</v>
+        <v>1705</v>
       </c>
       <c r="EE26" s="2">
         <v>1230</v>
       </c>
       <c r="EF26" s="2">
-        <v>578</v>
+        <v>580</v>
       </c>
       <c r="EG26" s="2" t="s">
         <v>223</v>
       </c>
       <c r="EH26" s="2">
-        <v>46.16613418530351</v>
+        <v>46.325878594249204</v>
       </c>
       <c r="EI26" s="2" t="s">
         <v>223</v>
@@ -18243,19 +18243,19 @@
         <v>223</v>
       </c>
       <c r="EP26" s="2">
-        <v>32931</v>
+        <v>32937</v>
       </c>
       <c r="EQ26" s="2">
         <v>32884</v>
       </c>
       <c r="ER26" s="2">
-        <v>4.11466399441256</v>
+        <v>4.113914442723988</v>
       </c>
       <c r="ES26" s="2" t="s">
         <v>223</v>
       </c>
       <c r="ET26" s="2">
-        <v>20878</v>
+        <v>20930</v>
       </c>
       <c r="EU26" s="2" t="s">
         <v>223</v>
@@ -18267,13 +18267,13 @@
         <v>223</v>
       </c>
       <c r="EX26" s="2">
-        <v>5757925</v>
+        <v>5769308</v>
       </c>
       <c r="EY26" s="2" t="s">
         <v>223</v>
       </c>
       <c r="EZ26" s="2">
-        <v>4250560</v>
+        <v>4257362</v>
       </c>
       <c r="FA26" s="2" t="s">
         <v>223</v>
@@ -18285,31 +18285,31 @@
         <v>223</v>
       </c>
       <c r="FD26" s="2">
-        <v>4247228</v>
+        <v>4254030</v>
       </c>
       <c r="FE26" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FF26" s="2">
-        <v>915555</v>
+        <v>918373</v>
       </c>
       <c r="FG26" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FH26" s="2">
-        <v>595142</v>
+        <v>596905</v>
       </c>
       <c r="FI26" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FJ26" s="2">
-        <v>1510697</v>
+        <v>1515278</v>
       </c>
       <c r="FK26" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FL26" s="2">
-        <v>11.76011537095477</v>
+        <v>11.755300193252651</v>
       </c>
       <c r="FM26" s="2" t="s">
         <v>223</v>
@@ -18321,7 +18321,7 @@
         <v>223</v>
       </c>
       <c r="FP26" s="2">
-        <v>205093</v>
+        <v>205394</v>
       </c>
       <c r="FQ26" s="2" t="s">
         <v>223</v>
@@ -18333,49 +18333,49 @@
         <v>223</v>
       </c>
       <c r="FT26" s="2">
-        <v>204989</v>
+        <v>205290</v>
       </c>
       <c r="FU26" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FV26" s="2">
-        <v>489979</v>
+        <v>491067</v>
       </c>
       <c r="FW26" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FX26" s="2">
-        <v>427745</v>
+        <v>428678</v>
       </c>
       <c r="FY26" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FZ26" s="2">
-        <v>222756</v>
+        <v>223388</v>
       </c>
       <c r="GA26" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GB26" s="2">
-        <v>62130</v>
+        <v>62285</v>
       </c>
       <c r="GC26" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GD26" s="2">
-        <v>284886</v>
+        <v>285673</v>
       </c>
       <c r="GE26" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GF26" s="2">
-        <v>25.856230537816014</v>
+        <v>25.853795935558598</v>
       </c>
       <c r="GG26" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GH26" s="2">
-        <v>14.115057792790415</v>
+        <v>14.111087711909024</v>
       </c>
       <c r="GI26" s="2" t="s">
         <v>223</v>
@@ -18393,43 +18393,43 @@
         <v>223</v>
       </c>
       <c r="GN26" s="2">
-        <v>15001</v>
+        <v>15007</v>
       </c>
       <c r="GO26" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GP26" s="2">
-        <v>18541</v>
+        <v>18544</v>
       </c>
       <c r="GQ26" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GR26" s="2">
-        <v>4103</v>
+        <v>4104</v>
       </c>
       <c r="GS26" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GT26" s="2">
-        <v>8933</v>
+        <v>8935</v>
       </c>
       <c r="GU26" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GV26" s="2">
-        <v>11257</v>
+        <v>11275</v>
       </c>
       <c r="GW26" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GX26" s="2">
-        <v>4852</v>
+        <v>4866</v>
       </c>
       <c r="GY26" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GZ26" s="2">
-        <v>2761</v>
+        <v>2776</v>
       </c>
       <c r="HA26" s="2" t="s">
         <v>223</v>
@@ -18447,25 +18447,25 @@
         <v>223</v>
       </c>
       <c r="HF26" s="2">
-        <v>0.8694798352332599</v>
+        <v>0.8683229813664596</v>
       </c>
       <c r="HG26" s="2" t="s">
         <v>223</v>
       </c>
       <c r="HH26" s="2">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="HI26" s="2" t="s">
         <v>223</v>
       </c>
       <c r="HJ26" s="2">
-        <v>5387</v>
+        <v>5399</v>
       </c>
       <c r="HK26" s="2" t="s">
         <v>223</v>
       </c>
       <c r="HL26" s="2">
-        <v>2252</v>
+        <v>2264</v>
       </c>
       <c r="HM26" s="2" t="s">
         <v>223</v>
@@ -19818,7 +19818,7 @@
         <v>202516</v>
       </c>
       <c r="F29" s="2">
-        <v>22198</v>
+        <v>22205</v>
       </c>
       <c r="G29" s="2">
         <v>22437</v>
@@ -19830,25 +19830,25 @@
         <v>223</v>
       </c>
       <c r="J29" s="2">
-        <v>37633295.269999996</v>
+        <v>37686257.93000001</v>
       </c>
       <c r="K29" s="2">
         <v>35593557.92</v>
       </c>
       <c r="L29" s="2">
-        <v>476</v>
+        <v>483</v>
       </c>
       <c r="M29" s="2">
         <v>505</v>
       </c>
       <c r="N29" s="2">
-        <v>15331</v>
+        <v>15366</v>
       </c>
       <c r="O29" s="2">
         <v>14735</v>
       </c>
       <c r="P29" s="2">
-        <v>11.724000795386756</v>
+        <v>11.710207165294843</v>
       </c>
       <c r="Q29" s="2" t="s">
         <v>223</v>
@@ -19860,13 +19860,13 @@
         <v>223</v>
       </c>
       <c r="T29" s="2">
-        <v>4451222</v>
+        <v>4457350</v>
       </c>
       <c r="U29" s="2" t="s">
         <v>223</v>
       </c>
       <c r="V29" s="2">
-        <v>15325</v>
+        <v>15360</v>
       </c>
       <c r="W29" s="2" t="s">
         <v>223</v>
@@ -19878,7 +19878,7 @@
         <v>223</v>
       </c>
       <c r="Z29" s="2">
-        <v>229624</v>
+        <v>229963</v>
       </c>
       <c r="AA29" s="2" t="s">
         <v>223</v>
@@ -19902,19 +19902,19 @@
         <v>223</v>
       </c>
       <c r="AH29" s="2">
-        <v>69.06478061086584</v>
+        <v>69.20063048862869</v>
       </c>
       <c r="AI29" s="2">
         <v>65.67</v>
       </c>
       <c r="AJ29" s="2">
-        <v>16827</v>
+        <v>16865</v>
       </c>
       <c r="AK29" s="2" t="s">
         <v>223</v>
       </c>
       <c r="AL29" s="2">
-        <v>13565</v>
+        <v>13593</v>
       </c>
       <c r="AM29" s="2">
         <v>12943</v>
@@ -19926,31 +19926,31 @@
         <v>223</v>
       </c>
       <c r="AP29" s="2">
-        <v>12677</v>
+        <v>12699</v>
       </c>
       <c r="AQ29" s="2" t="s">
         <v>223</v>
       </c>
       <c r="AR29" s="2">
-        <v>11903</v>
+        <v>11929</v>
       </c>
       <c r="AS29" s="2" t="s">
         <v>223</v>
       </c>
       <c r="AT29" s="2">
-        <v>61.10910892873231</v>
+        <v>61.21594235532538</v>
       </c>
       <c r="AU29" s="2">
         <v>57.69</v>
       </c>
       <c r="AV29" s="2">
-        <v>2454.72</v>
+        <v>2452.57</v>
       </c>
       <c r="AW29" s="2">
         <v>2415.58</v>
       </c>
       <c r="AX29" s="2">
-        <v>9253</v>
+        <v>9266</v>
       </c>
       <c r="AY29" s="2" t="s">
         <v>223</v>
@@ -20004,13 +20004,13 @@
         <v>223</v>
       </c>
       <c r="BP29" s="2">
-        <v>37567795.91</v>
+        <v>37620758.56999999</v>
       </c>
       <c r="BQ29" s="2" t="s">
         <v>223</v>
       </c>
       <c r="BR29" s="2">
-        <v>24140158.86</v>
+        <v>24163036.290000003</v>
       </c>
       <c r="BS29" s="2" t="s">
         <v>223</v>
@@ -20022,43 +20022,43 @@
         <v>223</v>
       </c>
       <c r="BV29" s="2">
-        <v>24074659.500000004</v>
+        <v>24097536.93</v>
       </c>
       <c r="BW29" s="2">
         <v>22681283.19</v>
       </c>
       <c r="BX29" s="2">
-        <v>7149383.100000001</v>
+        <v>7165893.3999999985</v>
       </c>
       <c r="BY29" s="2">
         <v>7687772.962</v>
       </c>
       <c r="BZ29" s="2">
-        <v>5241906.299999999</v>
+        <v>5252301.229999999</v>
       </c>
       <c r="CA29" s="2">
         <v>5224501.766</v>
       </c>
       <c r="CB29" s="2">
-        <v>103.40209333124513</v>
+        <v>103.39023588153799</v>
       </c>
       <c r="CC29" s="2" t="s">
         <v>223</v>
       </c>
       <c r="CD29" s="2">
-        <v>12391289.399999999</v>
+        <v>12418194.629999999</v>
       </c>
       <c r="CE29" s="2" t="s">
         <v>223</v>
       </c>
       <c r="CF29" s="2">
-        <v>8.454598595621606</v>
+        <v>8.454857242531999</v>
       </c>
       <c r="CG29" s="2" t="s">
         <v>223</v>
       </c>
       <c r="CH29" s="2">
-        <v>163.89094898616867</v>
+        <v>163.87965859725264</v>
       </c>
       <c r="CI29" s="2" t="s">
         <v>223</v>
@@ -20100,31 +20100,31 @@
         <v>223</v>
       </c>
       <c r="CV29" s="2">
-        <v>2454.7188878742413</v>
+        <v>2452.5743804503454</v>
       </c>
       <c r="CW29" s="2" t="s">
         <v>223</v>
       </c>
       <c r="CX29" s="2">
-        <v>289.81723305720436</v>
+        <v>289.55590264219705</v>
       </c>
       <c r="CY29" s="2" t="s">
         <v>223</v>
       </c>
       <c r="CZ29" s="2">
-        <v>19.384829111939517</v>
+        <v>19.38290072750834</v>
       </c>
       <c r="DA29" s="2" t="s">
         <v>223</v>
       </c>
       <c r="DB29" s="2">
-        <v>3338</v>
+        <v>3313</v>
       </c>
       <c r="DC29" s="2">
         <v>3973</v>
       </c>
       <c r="DD29" s="2">
-        <v>2105</v>
+        <v>2102</v>
       </c>
       <c r="DE29" s="2">
         <v>2069</v>
@@ -20136,13 +20136,13 @@
         <v>1304</v>
       </c>
       <c r="DH29" s="2">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="DI29" s="2">
         <v>983</v>
       </c>
       <c r="DJ29" s="2">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="DK29" s="2">
         <v>1092</v>
@@ -20154,7 +20154,7 @@
         <v>909</v>
       </c>
       <c r="DN29" s="2">
-        <v>2948</v>
+        <v>2945</v>
       </c>
       <c r="DO29" s="2" t="s">
         <v>223</v>
@@ -20196,13 +20196,13 @@
         <v>223</v>
       </c>
       <c r="EB29" s="2">
-        <v>994</v>
+        <v>998</v>
       </c>
       <c r="EC29" s="2" t="s">
         <v>223</v>
       </c>
       <c r="ED29" s="2">
-        <v>1112</v>
+        <v>1116</v>
       </c>
       <c r="EE29" s="2">
         <v>1207</v>
@@ -20226,7 +20226,7 @@
         <v>223</v>
       </c>
       <c r="EL29" s="2">
-        <v>654</v>
+        <v>657</v>
       </c>
       <c r="EM29" s="2">
         <v>585</v>
@@ -20238,19 +20238,19 @@
         <v>223</v>
       </c>
       <c r="EP29" s="2">
-        <v>25145</v>
+        <v>25149</v>
       </c>
       <c r="EQ29" s="2">
         <v>25421</v>
       </c>
       <c r="ER29" s="2">
-        <v>3.507655597534301</v>
+        <v>3.507097697721579</v>
       </c>
       <c r="ES29" s="2" t="s">
         <v>223</v>
       </c>
       <c r="ET29" s="2">
-        <v>16933</v>
+        <v>16971</v>
       </c>
       <c r="EU29" s="2" t="s">
         <v>223</v>
@@ -20262,13 +20262,13 @@
         <v>223</v>
       </c>
       <c r="EX29" s="2">
-        <v>4443188</v>
+        <v>4449316</v>
       </c>
       <c r="EY29" s="2" t="s">
         <v>223</v>
       </c>
       <c r="EZ29" s="2">
-        <v>2992864</v>
+        <v>2995522</v>
       </c>
       <c r="FA29" s="2" t="s">
         <v>223</v>
@@ -20280,31 +20280,31 @@
         <v>223</v>
       </c>
       <c r="FD29" s="2">
-        <v>2984830</v>
+        <v>2987488</v>
       </c>
       <c r="FE29" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FF29" s="2">
-        <v>898068</v>
+        <v>900437</v>
       </c>
       <c r="FG29" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FH29" s="2">
-        <v>560457</v>
+        <v>561558</v>
       </c>
       <c r="FI29" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FJ29" s="2">
-        <v>1458525</v>
+        <v>1461995</v>
       </c>
       <c r="FK29" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FL29" s="2">
-        <v>12.23027825174268</v>
+        <v>12.228501666643805</v>
       </c>
       <c r="FM29" s="2" t="s">
         <v>223</v>
@@ -20316,7 +20316,7 @@
         <v>223</v>
       </c>
       <c r="FP29" s="2">
-        <v>143963</v>
+        <v>144089</v>
       </c>
       <c r="FQ29" s="2" t="s">
         <v>223</v>
@@ -20328,49 +20328,49 @@
         <v>223</v>
       </c>
       <c r="FT29" s="2">
-        <v>143498</v>
+        <v>143624</v>
       </c>
       <c r="FU29" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FV29" s="2">
-        <v>363953</v>
+        <v>364527</v>
       </c>
       <c r="FW29" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FX29" s="2">
-        <v>305956</v>
+        <v>306405</v>
       </c>
       <c r="FY29" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FZ29" s="2">
-        <v>162458</v>
+        <v>162781</v>
       </c>
       <c r="GA29" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GB29" s="2">
-        <v>57532</v>
+        <v>57657</v>
       </c>
       <c r="GC29" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GD29" s="2">
-        <v>219990</v>
+        <v>220438</v>
       </c>
       <c r="GE29" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GF29" s="2">
-        <v>23.73954732241863</v>
+        <v>23.721528048939216</v>
       </c>
       <c r="GG29" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GH29" s="2">
-        <v>14.97775748483465</v>
+        <v>14.965703501236495</v>
       </c>
       <c r="GI29" s="2" t="s">
         <v>223</v>
@@ -20388,19 +20388,19 @@
         <v>223</v>
       </c>
       <c r="GN29" s="2">
-        <v>11493</v>
+        <v>11497</v>
       </c>
       <c r="GO29" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GP29" s="2">
-        <v>11754</v>
+        <v>11756</v>
       </c>
       <c r="GQ29" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GR29" s="2">
-        <v>4369</v>
+        <v>4371</v>
       </c>
       <c r="GS29" s="2" t="s">
         <v>223</v>
@@ -20412,19 +20412,19 @@
         <v>223</v>
       </c>
       <c r="GV29" s="2">
-        <v>7376</v>
+        <v>7389</v>
       </c>
       <c r="GW29" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GX29" s="2">
-        <v>4743</v>
+        <v>4750</v>
       </c>
       <c r="GY29" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GZ29" s="2">
-        <v>3153</v>
+        <v>3167</v>
       </c>
       <c r="HA29" s="2" t="s">
         <v>223</v>
@@ -20442,25 +20442,25 @@
         <v>223</v>
       </c>
       <c r="HF29" s="2">
-        <v>0.8636390480127561</v>
+        <v>0.8622355783395204</v>
       </c>
       <c r="HG29" s="2" t="s">
         <v>223</v>
       </c>
       <c r="HH29" s="2">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="HI29" s="2" t="s">
         <v>223</v>
       </c>
       <c r="HJ29" s="2">
-        <v>3424</v>
+        <v>3433</v>
       </c>
       <c r="HK29" s="2" t="s">
         <v>223</v>
       </c>
       <c r="HL29" s="2">
-        <v>2650</v>
+        <v>2663</v>
       </c>
       <c r="HM29" s="2" t="s">
         <v>223</v>
@@ -20483,7 +20483,7 @@
         <v>202516</v>
       </c>
       <c r="F30" s="2">
-        <v>22241</v>
+        <v>22275</v>
       </c>
       <c r="G30" s="2">
         <v>22703</v>
@@ -20495,25 +20495,25 @@
         <v>223</v>
       </c>
       <c r="J30" s="2">
-        <v>32592592.08</v>
+        <v>32946179.530000005</v>
       </c>
       <c r="K30" s="2">
         <v>35130008.8</v>
       </c>
       <c r="L30" s="2">
-        <v>283</v>
+        <v>317</v>
       </c>
       <c r="M30" s="2">
         <v>289</v>
       </c>
       <c r="N30" s="2">
-        <v>12308</v>
+        <v>12498</v>
       </c>
       <c r="O30" s="2">
         <v>14434</v>
       </c>
       <c r="P30" s="2">
-        <v>13.68751940391183</v>
+        <v>13.639359516147792</v>
       </c>
       <c r="Q30" s="2" t="s">
         <v>223</v>
@@ -20525,13 +20525,13 @@
         <v>223</v>
       </c>
       <c r="T30" s="2">
-        <v>3919761</v>
+        <v>3959988</v>
       </c>
       <c r="U30" s="2" t="s">
         <v>223</v>
       </c>
       <c r="V30" s="2">
-        <v>12303</v>
+        <v>12493</v>
       </c>
       <c r="W30" s="2" t="s">
         <v>223</v>
@@ -20543,7 +20543,7 @@
         <v>223</v>
       </c>
       <c r="Z30" s="2">
-        <v>174106</v>
+        <v>176349</v>
       </c>
       <c r="AA30" s="2" t="s">
         <v>223</v>
@@ -20567,19 +20567,19 @@
         <v>223</v>
       </c>
       <c r="AH30" s="2">
-        <v>55.33923834359966</v>
+        <v>56.107744107744104</v>
       </c>
       <c r="AI30" s="2">
         <v>63.58</v>
       </c>
       <c r="AJ30" s="2">
-        <v>13630</v>
+        <v>13827</v>
       </c>
       <c r="AK30" s="2" t="s">
         <v>223</v>
       </c>
       <c r="AL30" s="2">
-        <v>10533</v>
+        <v>10690</v>
       </c>
       <c r="AM30" s="2">
         <v>12631</v>
@@ -20591,31 +20591,31 @@
         <v>223</v>
       </c>
       <c r="AP30" s="2">
-        <v>10438</v>
+        <v>10569</v>
       </c>
       <c r="AQ30" s="2" t="s">
         <v>223</v>
       </c>
       <c r="AR30" s="2">
-        <v>9079</v>
+        <v>9224</v>
       </c>
       <c r="AS30" s="2" t="s">
         <v>223</v>
       </c>
       <c r="AT30" s="2">
-        <v>47.358482082640165</v>
+        <v>47.99102132435466</v>
       </c>
       <c r="AU30" s="2">
         <v>55.64</v>
       </c>
       <c r="AV30" s="2">
-        <v>2648.08</v>
+        <v>2636.12</v>
       </c>
       <c r="AW30" s="2">
         <v>2433.84</v>
       </c>
       <c r="AX30" s="2">
-        <v>7214</v>
+        <v>7300</v>
       </c>
       <c r="AY30" s="2" t="s">
         <v>223</v>
@@ -20669,13 +20669,13 @@
         <v>223</v>
       </c>
       <c r="BP30" s="2">
-        <v>32584195.67</v>
+        <v>32937783.12</v>
       </c>
       <c r="BQ30" s="2" t="s">
         <v>223</v>
       </c>
       <c r="BR30" s="2">
-        <v>22582499.57</v>
+        <v>22788102.770000003</v>
       </c>
       <c r="BS30" s="2" t="s">
         <v>223</v>
@@ -20687,43 +20687,43 @@
         <v>223</v>
       </c>
       <c r="BV30" s="2">
-        <v>22574103.160000004</v>
+        <v>22779706.360000003</v>
       </c>
       <c r="BW30" s="2">
         <v>23663087.41</v>
       </c>
       <c r="BX30" s="2">
-        <v>5524644.4399999995</v>
+        <v>5607517.6</v>
       </c>
       <c r="BY30" s="2">
         <v>6931597.166</v>
       </c>
       <c r="BZ30" s="2">
-        <v>3645273.6599999997</v>
+        <v>3695689.7499999995</v>
       </c>
       <c r="CA30" s="2">
         <v>4535324.225</v>
       </c>
       <c r="CB30" s="2">
-        <v>89.91109490259257</v>
+        <v>89.72002344701005</v>
       </c>
       <c r="CC30" s="2" t="s">
         <v>223</v>
       </c>
       <c r="CD30" s="2">
-        <v>9169918.100000001</v>
+        <v>9303207.35</v>
       </c>
       <c r="CE30" s="2" t="s">
         <v>223</v>
       </c>
       <c r="CF30" s="2">
-        <v>8.314943712129388</v>
+        <v>8.319767516972275</v>
       </c>
       <c r="CG30" s="2" t="s">
         <v>223</v>
       </c>
       <c r="CH30" s="2">
-        <v>187.19970638576498</v>
+        <v>186.8237388927638</v>
       </c>
       <c r="CI30" s="2" t="s">
         <v>223</v>
@@ -20765,61 +20765,61 @@
         <v>223</v>
       </c>
       <c r="CV30" s="2">
-        <v>2648.0819044523887</v>
+        <v>2636.1161409825577</v>
       </c>
       <c r="CW30" s="2" t="s">
         <v>223</v>
       </c>
       <c r="CX30" s="2">
-        <v>318.38885277868053</v>
+        <v>316.7672427588414</v>
       </c>
       <c r="CY30" s="2" t="s">
         <v>223</v>
       </c>
       <c r="CZ30" s="2">
-        <v>22.51364685881015</v>
+        <v>22.455403773199734</v>
       </c>
       <c r="DA30" s="2" t="s">
         <v>223</v>
       </c>
       <c r="DB30" s="2">
-        <v>4949</v>
+        <v>4826</v>
       </c>
       <c r="DC30" s="2">
         <v>3285</v>
       </c>
       <c r="DD30" s="2">
-        <v>2925</v>
+        <v>2906</v>
       </c>
       <c r="DE30" s="2">
         <v>2857</v>
       </c>
       <c r="DF30" s="2">
-        <v>2059</v>
+        <v>2045</v>
       </c>
       <c r="DG30" s="2">
         <v>1766</v>
       </c>
       <c r="DH30" s="2">
-        <v>1197</v>
+        <v>1192</v>
       </c>
       <c r="DI30" s="2">
         <v>1143</v>
       </c>
       <c r="DJ30" s="2">
-        <v>1212</v>
+        <v>1210</v>
       </c>
       <c r="DK30" s="2">
         <v>1186</v>
       </c>
       <c r="DL30" s="2">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="DM30" s="2">
         <v>1117</v>
       </c>
       <c r="DN30" s="2">
-        <v>3527</v>
+        <v>3518</v>
       </c>
       <c r="DO30" s="2" t="s">
         <v>223</v>
@@ -20861,37 +20861,37 @@
         <v>223</v>
       </c>
       <c r="EB30" s="2">
-        <v>1101</v>
+        <v>1125</v>
       </c>
       <c r="EC30" s="2" t="s">
         <v>223</v>
       </c>
       <c r="ED30" s="2">
-        <v>1209</v>
+        <v>1234</v>
       </c>
       <c r="EE30" s="2">
         <v>1097</v>
       </c>
       <c r="EF30" s="2">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="EG30" s="2" t="s">
         <v>223</v>
       </c>
       <c r="EH30" s="2">
-        <v>44.84389782403028</v>
+        <v>45.033112582781456</v>
       </c>
       <c r="EI30" s="2" t="s">
         <v>223</v>
       </c>
       <c r="EJ30" s="2">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="EK30" s="2" t="s">
         <v>223</v>
       </c>
       <c r="EL30" s="2">
-        <v>563</v>
+        <v>572</v>
       </c>
       <c r="EM30" s="2">
         <v>706</v>
@@ -20903,19 +20903,19 @@
         <v>223</v>
       </c>
       <c r="EP30" s="2">
-        <v>25768</v>
+        <v>25793</v>
       </c>
       <c r="EQ30" s="2">
         <v>26149</v>
       </c>
       <c r="ER30" s="2">
-        <v>4.338714684880472</v>
+        <v>4.326755321211182</v>
       </c>
       <c r="ES30" s="2" t="s">
         <v>223</v>
       </c>
       <c r="ET30" s="2">
-        <v>13642</v>
+        <v>13839</v>
       </c>
       <c r="EU30" s="2" t="s">
         <v>223</v>
@@ -20927,13 +20927,13 @@
         <v>223</v>
       </c>
       <c r="EX30" s="2">
-        <v>3918730</v>
+        <v>3958957</v>
       </c>
       <c r="EY30" s="2" t="s">
         <v>223</v>
       </c>
       <c r="EZ30" s="2">
-        <v>2796110</v>
+        <v>2820314</v>
       </c>
       <c r="FA30" s="2" t="s">
         <v>223</v>
@@ -20945,31 +20945,31 @@
         <v>223</v>
       </c>
       <c r="FD30" s="2">
-        <v>2795079</v>
+        <v>2819283</v>
       </c>
       <c r="FE30" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FF30" s="2">
-        <v>729818</v>
+        <v>740449</v>
       </c>
       <c r="FG30" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FH30" s="2">
-        <v>393833</v>
+        <v>399225</v>
       </c>
       <c r="FI30" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FJ30" s="2">
-        <v>1123651</v>
+        <v>1139674</v>
       </c>
       <c r="FK30" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FL30" s="2">
-        <v>10.813193452101805</v>
+        <v>10.783957996900964</v>
       </c>
       <c r="FM30" s="2" t="s">
         <v>223</v>
@@ -20981,7 +20981,7 @@
         <v>223</v>
       </c>
       <c r="FP30" s="2">
-        <v>129891</v>
+        <v>131144</v>
       </c>
       <c r="FQ30" s="2" t="s">
         <v>223</v>
@@ -20993,55 +20993,55 @@
         <v>223</v>
       </c>
       <c r="FT30" s="2">
-        <v>129831</v>
+        <v>131084</v>
       </c>
       <c r="FU30" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FV30" s="2">
-        <v>362498</v>
+        <v>367211</v>
       </c>
       <c r="FW30" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FX30" s="2">
-        <v>324666</v>
+        <v>328835</v>
       </c>
       <c r="FY30" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FZ30" s="2">
-        <v>194835</v>
+        <v>197751</v>
       </c>
       <c r="GA30" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GB30" s="2">
-        <v>37772</v>
+        <v>38316</v>
       </c>
       <c r="GC30" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GD30" s="2">
-        <v>232607</v>
+        <v>236067</v>
       </c>
       <c r="GE30" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GF30" s="2">
-        <v>29.45222619434514</v>
+        <v>29.381581052968475</v>
       </c>
       <c r="GG30" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GH30" s="2">
-        <v>14.1457588560286</v>
+        <v>14.110177628420548</v>
       </c>
       <c r="GI30" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GJ30" s="2">
-        <v>9292</v>
+        <v>9293</v>
       </c>
       <c r="GK30" s="2" t="s">
         <v>223</v>
@@ -21053,19 +21053,19 @@
         <v>223</v>
       </c>
       <c r="GN30" s="2">
-        <v>13273</v>
+        <v>13297</v>
       </c>
       <c r="GO30" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GP30" s="2">
-        <v>13381</v>
+        <v>13394</v>
       </c>
       <c r="GQ30" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GR30" s="2">
-        <v>4724</v>
+        <v>4736</v>
       </c>
       <c r="GS30" s="2" t="s">
         <v>223</v>
@@ -21077,19 +21077,19 @@
         <v>223</v>
       </c>
       <c r="GV30" s="2">
-        <v>6739</v>
+        <v>6811</v>
       </c>
       <c r="GW30" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GX30" s="2">
-        <v>3213</v>
+        <v>3262</v>
       </c>
       <c r="GY30" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GZ30" s="2">
-        <v>2301</v>
+        <v>2367</v>
       </c>
       <c r="HA30" s="2" t="s">
         <v>223</v>
@@ -21107,25 +21107,25 @@
         <v>223</v>
       </c>
       <c r="HF30" s="2">
-        <v>0.8808092655035918</v>
+        <v>0.8788207240407544</v>
       </c>
       <c r="HG30" s="2" t="s">
         <v>223</v>
       </c>
       <c r="HH30" s="2">
-        <v>-111</v>
+        <v>-84</v>
       </c>
       <c r="HI30" s="2" t="s">
         <v>223</v>
       </c>
       <c r="HJ30" s="2">
-        <v>3224</v>
+        <v>3269</v>
       </c>
       <c r="HK30" s="2" t="s">
         <v>223</v>
       </c>
       <c r="HL30" s="2">
-        <v>1865</v>
+        <v>1924</v>
       </c>
       <c r="HM30" s="2" t="s">
         <v>223</v>
@@ -23808,7 +23808,7 @@
         <v>202516</v>
       </c>
       <c r="F35" s="2">
-        <v>20072</v>
+        <v>20112</v>
       </c>
       <c r="G35" s="2">
         <v>20576</v>
@@ -23820,25 +23820,25 @@
         <v>223</v>
       </c>
       <c r="J35" s="2">
-        <v>31034820.500000004</v>
+        <v>31445985.56</v>
       </c>
       <c r="K35" s="2">
         <v>32779437.9</v>
       </c>
       <c r="L35" s="2">
-        <v>355</v>
+        <v>395</v>
       </c>
       <c r="M35" s="2">
         <v>590</v>
       </c>
       <c r="N35" s="2">
-        <v>11399</v>
+        <v>11618</v>
       </c>
       <c r="O35" s="2">
         <v>13557</v>
       </c>
       <c r="P35" s="2">
-        <v>13.138307079799203</v>
+        <v>13.05550752204738</v>
       </c>
       <c r="Q35" s="2" t="s">
         <v>223</v>
@@ -23850,13 +23850,13 @@
         <v>223</v>
       </c>
       <c r="T35" s="2">
-        <v>3733911</v>
+        <v>3781051</v>
       </c>
       <c r="U35" s="2" t="s">
         <v>223</v>
       </c>
       <c r="V35" s="2">
-        <v>11388</v>
+        <v>11607</v>
       </c>
       <c r="W35" s="2" t="s">
         <v>223</v>
@@ -23868,7 +23868,7 @@
         <v>223</v>
       </c>
       <c r="Z35" s="2">
-        <v>166905</v>
+        <v>169414</v>
       </c>
       <c r="AA35" s="2" t="s">
         <v>223</v>
@@ -23892,19 +23892,19 @@
         <v>223</v>
       </c>
       <c r="AH35" s="2">
-        <v>56.79055400557991</v>
+        <v>57.766507557677</v>
       </c>
       <c r="AI35" s="2">
         <v>65.89</v>
       </c>
       <c r="AJ35" s="2">
-        <v>12626</v>
+        <v>12865</v>
       </c>
       <c r="AK35" s="2" t="s">
         <v>223</v>
       </c>
       <c r="AL35" s="2">
-        <v>9898</v>
+        <v>10077</v>
       </c>
       <c r="AM35" s="2">
         <v>11793</v>
@@ -23916,31 +23916,31 @@
         <v>223</v>
       </c>
       <c r="AP35" s="2">
-        <v>9225</v>
+        <v>9372</v>
       </c>
       <c r="AQ35" s="2" t="s">
         <v>223</v>
       </c>
       <c r="AR35" s="2">
-        <v>8651</v>
+        <v>8827</v>
       </c>
       <c r="AS35" s="2" t="s">
         <v>223</v>
       </c>
       <c r="AT35" s="2">
-        <v>49.31247508967716</v>
+        <v>50.10441527446301</v>
       </c>
       <c r="AU35" s="2">
         <v>57.31</v>
       </c>
       <c r="AV35" s="2">
-        <v>2722.59</v>
+        <v>2706.66</v>
       </c>
       <c r="AW35" s="2">
         <v>2417.9</v>
       </c>
       <c r="AX35" s="2">
-        <v>6483</v>
+        <v>6585</v>
       </c>
       <c r="AY35" s="2" t="s">
         <v>223</v>
@@ -23994,13 +23994,13 @@
         <v>223</v>
       </c>
       <c r="BP35" s="2">
-        <v>30963353.84000001</v>
+        <v>31374518.900000002</v>
       </c>
       <c r="BQ35" s="2" t="s">
         <v>223</v>
       </c>
       <c r="BR35" s="2">
-        <v>19905977.259999998</v>
+        <v>20121910.67</v>
       </c>
       <c r="BS35" s="2" t="s">
         <v>223</v>
@@ -24012,43 +24012,43 @@
         <v>223</v>
       </c>
       <c r="BV35" s="2">
-        <v>19834510.599999998</v>
+        <v>20050444.009999998</v>
       </c>
       <c r="BW35" s="2">
         <v>20662215.29</v>
       </c>
       <c r="BX35" s="2">
-        <v>6567731.669999999</v>
+        <v>6672052.749999999</v>
       </c>
       <c r="BY35" s="2">
         <v>7380247.972</v>
       </c>
       <c r="BZ35" s="2">
-        <v>3787943.41</v>
+        <v>3863682.08</v>
       </c>
       <c r="CA35" s="2">
         <v>4736974.642</v>
       </c>
       <c r="CB35" s="2">
-        <v>86.42172850026037</v>
+        <v>86.30826705457739</v>
       </c>
       <c r="CC35" s="2" t="s">
         <v>223</v>
       </c>
       <c r="CD35" s="2">
-        <v>10355675.08</v>
+        <v>10535734.829999998</v>
       </c>
       <c r="CE35" s="2" t="s">
         <v>223</v>
       </c>
       <c r="CF35" s="2">
-        <v>8.311612274636435</v>
+        <v>8.316731395582869</v>
       </c>
       <c r="CG35" s="2" t="s">
         <v>223</v>
       </c>
       <c r="CH35" s="2">
-        <v>185.94302447500078</v>
+        <v>185.61621566104336</v>
       </c>
       <c r="CI35" s="2" t="s">
         <v>223</v>
@@ -24090,61 +24090,61 @@
         <v>223</v>
       </c>
       <c r="CV35" s="2">
-        <v>2722.5914992543208</v>
+        <v>2706.660833189878</v>
       </c>
       <c r="CW35" s="2" t="s">
         <v>223</v>
       </c>
       <c r="CX35" s="2">
-        <v>326.7975260987806</v>
+        <v>324.69487002926496</v>
       </c>
       <c r="CY35" s="2" t="s">
         <v>223</v>
       </c>
       <c r="CZ35" s="2">
-        <v>22.3714747910488</v>
+        <v>22.318409340432314</v>
       </c>
       <c r="DA35" s="2" t="s">
         <v>223</v>
       </c>
       <c r="DB35" s="2">
-        <v>4623</v>
+        <v>4480</v>
       </c>
       <c r="DC35" s="2">
         <v>2883</v>
       </c>
       <c r="DD35" s="2">
-        <v>2392</v>
+        <v>2371</v>
       </c>
       <c r="DE35" s="2">
         <v>2340</v>
       </c>
       <c r="DF35" s="2">
-        <v>1658</v>
+        <v>1643</v>
       </c>
       <c r="DG35" s="2">
         <v>1473</v>
       </c>
       <c r="DH35" s="2">
-        <v>929</v>
+        <v>921</v>
       </c>
       <c r="DI35" s="2">
         <v>891</v>
       </c>
       <c r="DJ35" s="2">
-        <v>1075</v>
+        <v>1071</v>
       </c>
       <c r="DK35" s="2">
         <v>1090</v>
       </c>
       <c r="DL35" s="2">
-        <v>1032</v>
+        <v>1028</v>
       </c>
       <c r="DM35" s="2">
         <v>1040</v>
       </c>
       <c r="DN35" s="2">
-        <v>3036</v>
+        <v>3020</v>
       </c>
       <c r="DO35" s="2" t="s">
         <v>223</v>
@@ -24186,37 +24186,37 @@
         <v>223</v>
       </c>
       <c r="EB35" s="2">
-        <v>902</v>
+        <v>924</v>
       </c>
       <c r="EC35" s="2" t="s">
         <v>223</v>
       </c>
       <c r="ED35" s="2">
-        <v>1008</v>
+        <v>1032</v>
       </c>
       <c r="EE35" s="2">
         <v>1187</v>
       </c>
       <c r="EF35" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="EG35" s="2" t="s">
         <v>223</v>
       </c>
       <c r="EH35" s="2">
-        <v>40.125</v>
+        <v>40.25</v>
       </c>
       <c r="EI35" s="2" t="s">
         <v>223</v>
       </c>
       <c r="EJ35" s="2">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="EK35" s="2" t="s">
         <v>223</v>
       </c>
       <c r="EL35" s="2">
-        <v>492</v>
+        <v>508</v>
       </c>
       <c r="EM35" s="2">
         <v>577</v>
@@ -24228,19 +24228,19 @@
         <v>223</v>
       </c>
       <c r="EP35" s="2">
-        <v>23108</v>
+        <v>23132</v>
       </c>
       <c r="EQ35" s="2">
         <v>23597</v>
       </c>
       <c r="ER35" s="2">
-        <v>4.465985805781548</v>
+        <v>4.444060176379042</v>
       </c>
       <c r="ES35" s="2" t="s">
         <v>223</v>
       </c>
       <c r="ET35" s="2">
-        <v>12743</v>
+        <v>12982</v>
       </c>
       <c r="EU35" s="2" t="s">
         <v>223</v>
@@ -24252,13 +24252,13 @@
         <v>223</v>
       </c>
       <c r="EX35" s="2">
-        <v>3725165</v>
+        <v>3772305</v>
       </c>
       <c r="EY35" s="2" t="s">
         <v>223</v>
       </c>
       <c r="EZ35" s="2">
-        <v>2468354</v>
+        <v>2493813</v>
       </c>
       <c r="FA35" s="2" t="s">
         <v>223</v>
@@ -24270,31 +24270,31 @@
         <v>223</v>
       </c>
       <c r="FD35" s="2">
-        <v>2459608</v>
+        <v>2485067</v>
       </c>
       <c r="FE35" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FF35" s="2">
-        <v>858143</v>
+        <v>872073</v>
       </c>
       <c r="FG35" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FH35" s="2">
-        <v>407297</v>
+        <v>415401</v>
       </c>
       <c r="FI35" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FJ35" s="2">
-        <v>1265440</v>
+        <v>1287474</v>
       </c>
       <c r="FK35" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FL35" s="2">
-        <v>10.397709330593218</v>
+        <v>10.377666771878301</v>
       </c>
       <c r="FM35" s="2" t="s">
         <v>223</v>
@@ -24306,7 +24306,7 @@
         <v>223</v>
       </c>
       <c r="FP35" s="2">
-        <v>114025</v>
+        <v>115314</v>
       </c>
       <c r="FQ35" s="2" t="s">
         <v>223</v>
@@ -24318,49 +24318,49 @@
         <v>223</v>
       </c>
       <c r="FT35" s="2">
-        <v>113520</v>
+        <v>114809</v>
       </c>
       <c r="FU35" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FV35" s="2">
-        <v>359109</v>
+        <v>364461</v>
       </c>
       <c r="FW35" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FX35" s="2">
-        <v>319310</v>
+        <v>323968</v>
       </c>
       <c r="FY35" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FZ35" s="2">
-        <v>205790</v>
+        <v>209159</v>
       </c>
       <c r="GA35" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GB35" s="2">
-        <v>39294</v>
+        <v>39988</v>
       </c>
       <c r="GC35" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GD35" s="2">
-        <v>245084</v>
+        <v>249147</v>
       </c>
       <c r="GE35" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GF35" s="2">
-        <v>31.503552943240635</v>
+        <v>31.360389051471856</v>
       </c>
       <c r="GG35" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GH35" s="2">
-        <v>14.642073866128607</v>
+        <v>14.582027887760372</v>
       </c>
       <c r="GI35" s="2" t="s">
         <v>223</v>
@@ -24372,49 +24372,49 @@
         <v>223</v>
       </c>
       <c r="GL35" s="2">
-        <v>3981</v>
+        <v>3982</v>
       </c>
       <c r="GM35" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GN35" s="2">
-        <v>11041</v>
+        <v>11064</v>
       </c>
       <c r="GO35" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GP35" s="2">
-        <v>11291</v>
+        <v>11303</v>
       </c>
       <c r="GQ35" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GR35" s="2">
-        <v>5285</v>
+        <v>5299</v>
       </c>
       <c r="GS35" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GT35" s="2">
-        <v>6532</v>
+        <v>6530</v>
       </c>
       <c r="GU35" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GV35" s="2">
-        <v>5765</v>
+        <v>5851</v>
       </c>
       <c r="GW35" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GX35" s="2">
-        <v>2914</v>
+        <v>2965</v>
       </c>
       <c r="GY35" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GZ35" s="2">
-        <v>2668</v>
+        <v>2748</v>
       </c>
       <c r="HA35" s="2" t="s">
         <v>223</v>
@@ -24432,25 +24432,25 @@
         <v>223</v>
       </c>
       <c r="HF35" s="2">
-        <v>0.8850349211331712</v>
+        <v>0.8826066861808658</v>
       </c>
       <c r="HG35" s="2" t="s">
         <v>223</v>
       </c>
       <c r="HH35" s="2">
-        <v>-70</v>
+        <v>-42</v>
       </c>
       <c r="HI35" s="2" t="s">
         <v>223</v>
       </c>
       <c r="HJ35" s="2">
-        <v>2742</v>
+        <v>2787</v>
       </c>
       <c r="HK35" s="2" t="s">
         <v>223</v>
       </c>
       <c r="HL35" s="2">
-        <v>2168</v>
+        <v>2242</v>
       </c>
       <c r="HM35" s="2" t="s">
         <v>223</v>
@@ -24473,7 +24473,7 @@
         <v>202516</v>
       </c>
       <c r="F36" s="2">
-        <v>34270</v>
+        <v>34334</v>
       </c>
       <c r="G36" s="2">
         <v>35500</v>
@@ -24485,25 +24485,25 @@
         <v>223</v>
       </c>
       <c r="J36" s="2">
-        <v>53155924.16</v>
+        <v>53693066.20000001</v>
       </c>
       <c r="K36" s="2">
         <v>59569249.18</v>
       </c>
       <c r="L36" s="2">
-        <v>80</v>
+        <v>136</v>
       </c>
       <c r="M36" s="2">
         <v>911</v>
       </c>
       <c r="N36" s="2">
-        <v>19490</v>
+        <v>19777</v>
       </c>
       <c r="O36" s="2">
         <v>23307</v>
       </c>
       <c r="P36" s="2">
-        <v>12.112430436232144</v>
+        <v>12.036277925804468</v>
       </c>
       <c r="Q36" s="2" t="s">
         <v>223</v>
@@ -24515,13 +24515,13 @@
         <v>223</v>
       </c>
       <c r="T36" s="2">
-        <v>6381964</v>
+        <v>6441605</v>
       </c>
       <c r="U36" s="2" t="s">
         <v>223</v>
       </c>
       <c r="V36" s="2">
-        <v>19468</v>
+        <v>19755</v>
       </c>
       <c r="W36" s="2" t="s">
         <v>223</v>
@@ -24533,7 +24533,7 @@
         <v>223</v>
       </c>
       <c r="Z36" s="2">
-        <v>294827</v>
+        <v>298317</v>
       </c>
       <c r="AA36" s="2" t="s">
         <v>223</v>
@@ -24557,19 +24557,19 @@
         <v>223</v>
       </c>
       <c r="AH36" s="2">
-        <v>56.87189962065947</v>
+        <v>57.60179413991962</v>
       </c>
       <c r="AI36" s="2">
         <v>65.65</v>
       </c>
       <c r="AJ36" s="2">
-        <v>21832</v>
+        <v>22133</v>
       </c>
       <c r="AK36" s="2" t="s">
         <v>223</v>
       </c>
       <c r="AL36" s="2">
-        <v>17355</v>
+        <v>17585</v>
       </c>
       <c r="AM36" s="2">
         <v>20311</v>
@@ -24581,31 +24581,31 @@
         <v>223</v>
       </c>
       <c r="AP36" s="2">
-        <v>17995</v>
+        <v>18235</v>
       </c>
       <c r="AQ36" s="2" t="s">
         <v>223</v>
       </c>
       <c r="AR36" s="2">
-        <v>13938</v>
+        <v>14155</v>
       </c>
       <c r="AS36" s="2" t="s">
         <v>223</v>
       </c>
       <c r="AT36" s="2">
-        <v>50.64196089874525</v>
+        <v>51.21745208830897</v>
       </c>
       <c r="AU36" s="2">
         <v>57.21</v>
       </c>
       <c r="AV36" s="2">
-        <v>2727.34</v>
+        <v>2714.92</v>
       </c>
       <c r="AW36" s="2">
         <v>2555.85</v>
       </c>
       <c r="AX36" s="2">
-        <v>12447</v>
+        <v>12614</v>
       </c>
       <c r="AY36" s="2" t="s">
         <v>223</v>
@@ -24659,13 +24659,13 @@
         <v>223</v>
       </c>
       <c r="BP36" s="2">
-        <v>52936496.42000001</v>
+        <v>53473638.46000001</v>
       </c>
       <c r="BQ36" s="2" t="s">
         <v>223</v>
       </c>
       <c r="BR36" s="2">
-        <v>39135109.370000005</v>
+        <v>39459463.11</v>
       </c>
       <c r="BS36" s="2" t="s">
         <v>223</v>
@@ -24677,43 +24677,43 @@
         <v>223</v>
       </c>
       <c r="BV36" s="2">
-        <v>38915681.63</v>
+        <v>39240035.37</v>
       </c>
       <c r="BW36" s="2">
         <v>42751146.92</v>
       </c>
       <c r="BX36" s="2">
-        <v>7432539.87</v>
+        <v>7554936.409999999</v>
       </c>
       <c r="BY36" s="2">
         <v>10352871.12</v>
       </c>
       <c r="BZ36" s="2">
-        <v>5270174.619999999</v>
+        <v>5339975.679999999</v>
       </c>
       <c r="CA36" s="2">
         <v>6465231.138</v>
       </c>
       <c r="CB36" s="2">
-        <v>123.64114374501361</v>
+        <v>123.46128563479255</v>
       </c>
       <c r="CC36" s="2" t="s">
         <v>223</v>
       </c>
       <c r="CD36" s="2">
-        <v>12702714.49</v>
+        <v>12894912.089999998</v>
       </c>
       <c r="CE36" s="2" t="s">
         <v>223</v>
       </c>
       <c r="CF36" s="2">
-        <v>8.329085554227508</v>
+        <v>8.335355272482559</v>
       </c>
       <c r="CG36" s="2" t="s">
         <v>223</v>
       </c>
       <c r="CH36" s="2">
-        <v>180.29530592516966</v>
+        <v>179.98661222793206</v>
       </c>
       <c r="CI36" s="2" t="s">
         <v>223</v>
@@ -24755,61 +24755,61 @@
         <v>223</v>
       </c>
       <c r="CV36" s="2">
-        <v>2727.343466393022</v>
+        <v>2714.9247206350815</v>
       </c>
       <c r="CW36" s="2" t="s">
         <v>223</v>
       </c>
       <c r="CX36" s="2">
-        <v>326.0653155464341</v>
+        <v>324.34919350760987</v>
       </c>
       <c r="CY36" s="2" t="s">
         <v>223</v>
       </c>
       <c r="CZ36" s="2">
-        <v>21.64647064210537</v>
+        <v>21.59315426207692</v>
       </c>
       <c r="DA36" s="2" t="s">
         <v>223</v>
       </c>
       <c r="DB36" s="2">
-        <v>8001</v>
+        <v>7818</v>
       </c>
       <c r="DC36" s="2">
         <v>5388</v>
       </c>
       <c r="DD36" s="2">
-        <v>4162</v>
+        <v>4139</v>
       </c>
       <c r="DE36" s="2">
         <v>4015</v>
       </c>
       <c r="DF36" s="2">
-        <v>2617</v>
+        <v>2600</v>
       </c>
       <c r="DG36" s="2">
         <v>2230</v>
       </c>
       <c r="DH36" s="2">
-        <v>1556</v>
+        <v>1546</v>
       </c>
       <c r="DI36" s="2">
         <v>1542</v>
       </c>
       <c r="DJ36" s="2">
-        <v>1896</v>
+        <v>1888</v>
       </c>
       <c r="DK36" s="2">
         <v>1956</v>
       </c>
       <c r="DL36" s="2">
-        <v>1271</v>
+        <v>1264</v>
       </c>
       <c r="DM36" s="2">
         <v>1293</v>
       </c>
       <c r="DN36" s="2">
-        <v>4723</v>
+        <v>4698</v>
       </c>
       <c r="DO36" s="2" t="s">
         <v>223</v>
@@ -24851,13 +24851,13 @@
         <v>223</v>
       </c>
       <c r="EB36" s="2">
-        <v>998</v>
+        <v>1026</v>
       </c>
       <c r="EC36" s="2" t="s">
         <v>223</v>
       </c>
       <c r="ED36" s="2">
-        <v>1122</v>
+        <v>1153</v>
       </c>
       <c r="EE36" s="2">
         <v>1919</v>
@@ -24875,13 +24875,13 @@
         <v>223</v>
       </c>
       <c r="EJ36" s="2">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="EK36" s="2" t="s">
         <v>223</v>
       </c>
       <c r="EL36" s="2">
-        <v>1013</v>
+        <v>1038</v>
       </c>
       <c r="EM36" s="2">
         <v>1077</v>
@@ -24893,19 +24893,19 @@
         <v>223</v>
       </c>
       <c r="EP36" s="2">
-        <v>38993</v>
+        <v>39032</v>
       </c>
       <c r="EQ36" s="2">
         <v>40291</v>
       </c>
       <c r="ER36" s="2">
-        <v>3.2595594080988897</v>
+        <v>3.2383685181389628</v>
       </c>
       <c r="ES36" s="2" t="s">
         <v>223</v>
       </c>
       <c r="ET36" s="2">
-        <v>21973</v>
+        <v>22274</v>
       </c>
       <c r="EU36" s="2" t="s">
         <v>223</v>
@@ -24917,13 +24917,13 @@
         <v>223</v>
       </c>
       <c r="EX36" s="2">
-        <v>6355013</v>
+        <v>6414654</v>
       </c>
       <c r="EY36" s="2" t="s">
         <v>223</v>
       </c>
       <c r="EZ36" s="2">
-        <v>4888089</v>
+        <v>4925791</v>
       </c>
       <c r="FA36" s="2" t="s">
         <v>223</v>
@@ -24935,31 +24935,31 @@
         <v>223</v>
       </c>
       <c r="FD36" s="2">
-        <v>4861138</v>
+        <v>4898840</v>
       </c>
       <c r="FE36" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FF36" s="2">
-        <v>924428</v>
+        <v>939276</v>
       </c>
       <c r="FG36" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FH36" s="2">
-        <v>569447</v>
+        <v>576925</v>
       </c>
       <c r="FI36" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FJ36" s="2">
-        <v>1493875</v>
+        <v>1516201</v>
       </c>
       <c r="FK36" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FL36" s="2">
-        <v>14.84450399026798</v>
+        <v>14.811760458774241</v>
       </c>
       <c r="FM36" s="2" t="s">
         <v>223</v>
@@ -24971,7 +24971,7 @@
         <v>223</v>
       </c>
       <c r="FP36" s="2">
-        <v>234028</v>
+        <v>236017</v>
       </c>
       <c r="FQ36" s="2" t="s">
         <v>223</v>
@@ -24983,49 +24983,49 @@
         <v>223</v>
       </c>
       <c r="FT36" s="2">
-        <v>233371</v>
+        <v>235360</v>
       </c>
       <c r="FU36" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FV36" s="2">
-        <v>429960</v>
+        <v>435045</v>
       </c>
       <c r="FW36" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FX36" s="2">
-        <v>373652</v>
+        <v>378003</v>
       </c>
       <c r="FY36" s="2" t="s">
         <v>223</v>
       </c>
       <c r="FZ36" s="2">
-        <v>140281</v>
+        <v>142643</v>
       </c>
       <c r="GA36" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GB36" s="2">
-        <v>55651</v>
+        <v>56385</v>
       </c>
       <c r="GC36" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GD36" s="2">
-        <v>195932</v>
+        <v>199028</v>
       </c>
       <c r="GE36" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GF36" s="2">
-        <v>22.058542842483323</v>
+        <v>21.990089497901604</v>
       </c>
       <c r="GG36" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GH36" s="2">
-        <v>15.127090815802976</v>
+        <v>15.08403701269151</v>
       </c>
       <c r="GI36" s="2" t="s">
         <v>223</v>
@@ -25037,49 +25037,49 @@
         <v>223</v>
       </c>
       <c r="GL36" s="2">
-        <v>3248</v>
+        <v>3251</v>
       </c>
       <c r="GM36" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GN36" s="2">
-        <v>17613</v>
+        <v>17652</v>
       </c>
       <c r="GO36" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GP36" s="2">
-        <v>23314</v>
+        <v>23332</v>
       </c>
       <c r="GQ36" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GR36" s="2">
-        <v>3261</v>
+        <v>3259</v>
       </c>
       <c r="GS36" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GT36" s="2">
-        <v>12418</v>
+        <v>12444</v>
       </c>
       <c r="GU36" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GV36" s="2">
-        <v>12019</v>
+        <v>12156</v>
       </c>
       <c r="GW36" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GX36" s="2">
-        <v>5518</v>
+        <v>5616</v>
       </c>
       <c r="GY36" s="2" t="s">
         <v>223</v>
       </c>
       <c r="GZ36" s="2">
-        <v>1914</v>
+        <v>1967</v>
       </c>
       <c r="HA36" s="2" t="s">
         <v>223</v>
@@ -25097,25 +25097,25 @@
         <v>223</v>
       </c>
       <c r="HF36" s="2">
-        <v>0.9224957902880808</v>
+        <v>0.9210738978180839</v>
       </c>
       <c r="HG36" s="2" t="s">
         <v>223</v>
       </c>
       <c r="HH36" s="2">
-        <v>-183</v>
+        <v>-145</v>
       </c>
       <c r="HI36" s="2" t="s">
         <v>223</v>
       </c>
       <c r="HJ36" s="2">
-        <v>5548</v>
+        <v>5621</v>
       </c>
       <c r="HK36" s="2" t="s">
         <v>223</v>
       </c>
       <c r="HL36" s="2">
-        <v>1491</v>
+        <v>1541</v>
       </c>
       <c r="HM36" s="2" t="s">
         <v>223</v>

</xml_diff>